<commit_message>
new paths and corrections
</commit_message>
<xml_diff>
--- a/data/Spis odcinków_KO-CB-KZ-KL.xlsx
+++ b/data/Spis odcinków_KO-CB-KZ-KL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\railways_dispatching_silesia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681DD843-1EB6-4A4F-910D-EA4C5DEA419A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6E5DBA-3A0F-455B-856F-4084B54F9D45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="517">
   <si>
     <t>Katowice</t>
   </si>
@@ -1029,9 +1029,6 @@
     <t>"CB-CM", "SBL+Sem(ST)", 1, "1", "(1)"</t>
   </si>
   <si>
-    <t>"CM-CB", "SBL+Sem(ST)", 1, "1", "(1)"</t>
-  </si>
-  <si>
     <t>"CM", "ST", 1, "(1)"</t>
   </si>
   <si>
@@ -1377,9 +1374,6 @@
     <t>"RCB-ZZ-1", "SBL", 1, "1", "(4)"</t>
   </si>
   <si>
-    <t>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</t>
-  </si>
-  <si>
     <t>"RCB-ZZ-3", "SBL", 1, "3", "(4)"</t>
   </si>
   <si>
@@ -1392,9 +1386,6 @@
     <t>"ZZ-RCB-2", "SBL", 2, "2", "(4)"</t>
   </si>
   <si>
-    <t>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</t>
-  </si>
-  <si>
     <t>"ZZ-RCB-4", "SBL+Sem(ST)", 2, "4", "(4)"</t>
   </si>
   <si>
@@ -1434,30 +1425,6 @@
     <t>"GLC-ZZ-5", "SBL+Sem(ST)", 2, "5", "(5)"</t>
   </si>
   <si>
-    <t>"GLC", "", 3, "(1)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 4, "(1)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 5, "(2)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 6, "(2)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 7, "(3)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 8, "(3)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 9, "(4)"</t>
-  </si>
-  <si>
-    <t>"GLC", "", 11, "(4)"</t>
-  </si>
-  <si>
     <t>"KL-MJ-1", "Sem(odstep)+PO(Piotrowice)", 1, "1", "(2)"</t>
   </si>
   <si>
@@ -1576,6 +1543,42 @@
   </si>
   <si>
     <t>"Ty", "ST", 108, "(N/A)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 3, "(1)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 4, "(1)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 5, "(2)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 6, "(2)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 7, "(3)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 8, "(3)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 9, "(4)"</t>
+  </si>
+  <si>
+    <t>"GLC", "ST", 11, "(4)"</t>
+  </si>
+  <si>
+    <t>"CM-CB", "SBL+Sem(ST)", 2, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"RCB-ZZ-2", "SBL+PO(Ruda Śląska)", 1, "2", "(4)"</t>
+  </si>
+  <si>
+    <t>"ZZ-RCB-3", "SBL+PO(Ruda Śląska)", 2, "3", "(4)"</t>
+  </si>
+  <si>
+    <t>"GLC(KS)", "B-M", 200, "(N/A)"</t>
   </si>
 </sst>
 </file>
@@ -2153,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM399"/>
+  <dimension ref="A1:AM400"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="M52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2419,7 @@
       </c>
       <c r="F6" s="17"/>
       <c r="L6" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(C6="",CONCATENATE($F$1,F6,$F$1,$G$1,$F$1,B6,$F$1,$G$1,G6,$G$1,$F$1,H6,$F$1,$G$1,$F$1,$B$1,I6,$C$1,$F$1),CONCATENATE($F$1,C6,$F$1,$G$1, $F$1,B6,$F$1,$G$1,D6,$G$1,$F$1,$B$1,E6,$C$1,$F$1))</f>
         <v>"KO", "ST", 2, "(3)"</v>
       </c>
       <c r="M6" s="20" t="s">
@@ -3041,7 +3044,7 @@
       </c>
       <c r="F23" s="17"/>
       <c r="L23" s="11" t="str">
-        <f t="shared" ref="L23:L134" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
+        <f t="shared" ref="L23:L135" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
         <v>"KO", "ST-M", 1114, "(N/A)"</v>
       </c>
       <c r="M23" s="11" t="s">
@@ -3524,7 +3527,7 @@
         <v>273</v>
       </c>
       <c r="N34" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
@@ -3752,7 +3755,7 @@
         <v>332</v>
       </c>
       <c r="N41" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O41" s="14"/>
       <c r="P41" s="14"/>
@@ -3785,10 +3788,10 @@
         <v>"CM-CB", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>333</v>
+        <v>513</v>
       </c>
       <c r="N42" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O42" s="14"/>
       <c r="P42" s="14"/>
@@ -3817,10 +3820,10 @@
         <v>"CM", "ST", 1, "(1)"</v>
       </c>
       <c r="M43" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N43" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
@@ -3849,10 +3852,10 @@
         <v>"CM", "ST", 2, "(1)"</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N44" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
@@ -3862,14 +3865,14 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B45" t="s">
         <v>67</v>
       </c>
       <c r="D45"/>
       <c r="F45" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>7</v>
@@ -3885,7 +3888,7 @@
         <v>"CB-RCB-1", "SBL", 1, "1", "(3)"</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N45" s="34">
         <v>137</v>
@@ -3898,14 +3901,14 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D46"/>
       <c r="F46" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>7</v>
@@ -3921,7 +3924,7 @@
         <v>"CB-RCB-2", "SBL+PO(Świętochłowice)", 1, "2", "(3)"</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N46" s="34">
         <v>137</v>
@@ -3934,14 +3937,14 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B47" t="s">
         <v>77</v>
       </c>
       <c r="D47"/>
       <c r="F47" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>7</v>
@@ -3957,7 +3960,7 @@
         <v>"CB-RCB-3", "SBL+Sem(ST)", 1, "3", "(3)"</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N47" s="34">
         <v>137</v>
@@ -3970,14 +3973,14 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B48" t="s">
         <v>67</v>
       </c>
       <c r="D48"/>
       <c r="F48" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>8</v>
@@ -3993,7 +3996,7 @@
         <v>"RCB-CB-1", "SBL", 2, "1", "(3)"</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N48" s="34">
         <v>137</v>
@@ -4006,14 +4009,14 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B49" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D49"/>
       <c r="F49" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>8</v>
@@ -4029,7 +4032,7 @@
         <v>"RCB-CB-2", "SBL+PO(Świętochłowice)", 2, "2", "(3)"</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N49" s="34">
         <v>137</v>
@@ -4042,14 +4045,14 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B50" t="s">
         <v>77</v>
       </c>
       <c r="D50"/>
       <c r="F50" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>8</v>
@@ -4065,7 +4068,7 @@
         <v>"RCB-CB-3", "SBL+Sem(ST)", 2, "3", "(3)"</v>
       </c>
       <c r="M50" s="20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N50" s="34">
         <v>137</v>
@@ -4078,13 +4081,13 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -4097,7 +4100,7 @@
         <v>"RCB", "ST", 1, "(1)"</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N51" s="34">
         <v>137</v>
@@ -4110,13 +4113,13 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -4129,7 +4132,7 @@
         <v>"RCB", "ST", 2, "(1)"</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N52" s="34">
         <v>137</v>
@@ -4142,14 +4145,14 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B53" t="s">
         <v>67</v>
       </c>
       <c r="D53"/>
       <c r="F53" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>7</v>
@@ -4165,7 +4168,7 @@
         <v>"RCB-ZZ-1", "SBL", 1, "1", "(4)"</v>
       </c>
       <c r="M53" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="N53" s="34">
         <v>137</v>
@@ -4178,14 +4181,14 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B54" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D54"/>
       <c r="F54" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>7</v>
@@ -4201,7 +4204,7 @@
         <v>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</v>
       </c>
       <c r="M54" s="20" t="s">
-        <v>449</v>
+        <v>514</v>
       </c>
       <c r="N54" s="34">
         <v>137</v>
@@ -4214,14 +4217,14 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B55" t="s">
         <v>67</v>
       </c>
       <c r="D55"/>
       <c r="F55" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>7</v>
@@ -4237,7 +4240,7 @@
         <v>"RCB-ZZ-3", "SBL", 1, "3", "(4)"</v>
       </c>
       <c r="M55" s="20" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="N55" s="34">
         <v>137</v>
@@ -4250,14 +4253,14 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B56" t="s">
         <v>77</v>
       </c>
       <c r="D56"/>
       <c r="F56" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>7</v>
@@ -4273,7 +4276,7 @@
         <v>"RCB-ZZ-4", "SBL+Sem(ST)", 1, "4", "(4)"</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="N56" s="34">
         <v>137</v>
@@ -4286,14 +4289,14 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B57" t="s">
         <v>67</v>
       </c>
       <c r="D57"/>
       <c r="F57" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>8</v>
@@ -4309,7 +4312,7 @@
         <v>"ZZ-RCB-1", "SBL", 2, "1", "(4)"</v>
       </c>
       <c r="M57" s="20" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="N57" s="34">
         <v>137</v>
@@ -4322,14 +4325,14 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B58" t="s">
         <v>67</v>
       </c>
       <c r="D58"/>
       <c r="F58" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>8</v>
@@ -4345,7 +4348,7 @@
         <v>"ZZ-RCB-2", "SBL", 2, "2", "(4)"</v>
       </c>
       <c r="M58" s="20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="N58" s="34">
         <v>137</v>
@@ -4358,14 +4361,14 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B59" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D59"/>
       <c r="F59" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>8</v>
@@ -4381,7 +4384,7 @@
         <v>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>454</v>
+        <v>515</v>
       </c>
       <c r="N59" s="34">
         <v>137</v>
@@ -4394,14 +4397,14 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B60" t="s">
         <v>77</v>
       </c>
       <c r="D60"/>
       <c r="F60" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>8</v>
@@ -4417,7 +4420,7 @@
         <v>"ZZ-RCB-4", "SBL+Sem(ST)", 2, "4", "(4)"</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="N60" s="34">
         <v>137</v>
@@ -4430,13 +4433,13 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B61" t="s">
         <v>20</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -4449,7 +4452,7 @@
         <v>"ZZ", "ST", 1, "(1)"</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="N61" s="34">
         <v>137</v>
@@ -4462,13 +4465,13 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B62" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -4481,7 +4484,7 @@
         <v>"ZZ", "ST", 2, "(1)"</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="N62" s="34">
         <v>137</v>
@@ -4494,14 +4497,14 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B63" t="s">
         <v>67</v>
       </c>
       <c r="D63"/>
       <c r="F63" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>7</v>
@@ -4517,7 +4520,7 @@
         <v>"ZZ-GLC-1", "SBL", 1, "1", "(5)"</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="N63" s="34">
         <v>137</v>
@@ -4530,14 +4533,14 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B64" t="s">
         <v>67</v>
       </c>
       <c r="D64"/>
       <c r="F64" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>7</v>
@@ -4553,7 +4556,7 @@
         <v>"ZZ-GLC-2", "SBL", 1, "2", "(5)"</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="N64" s="34">
         <v>137</v>
@@ -4566,14 +4569,14 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B65" t="s">
         <v>67</v>
       </c>
       <c r="D65"/>
       <c r="F65" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>7</v>
@@ -4589,7 +4592,7 @@
         <v>"ZZ-GLC-3", "SBL", 1, "3", "(5)"</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="N65" s="34"/>
       <c r="O65" s="14"/>
@@ -4600,14 +4603,14 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B66" t="s">
         <v>67</v>
       </c>
       <c r="D66"/>
       <c r="F66" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>7</v>
@@ -4623,7 +4626,7 @@
         <v>"ZZ-GLC-4", "SBL", 1, "4", "(5)"</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="N66" s="34"/>
       <c r="O66" s="14"/>
@@ -4634,14 +4637,14 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B67" t="s">
         <v>77</v>
       </c>
       <c r="D67"/>
       <c r="F67" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>7</v>
@@ -4657,7 +4660,7 @@
         <v>"ZZ-GLC-5", "SBL+Sem(ST)", 1, "5", "(5)"</v>
       </c>
       <c r="M67" s="20" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="N67" s="34"/>
       <c r="O67" s="14"/>
@@ -4668,14 +4671,14 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
       <c r="D68"/>
       <c r="F68" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>8</v>
@@ -4691,7 +4694,7 @@
         <v>"GLC-ZZ-1", "SBL", 2, "1", "(5)"</v>
       </c>
       <c r="M68" s="20" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="N68" s="34"/>
       <c r="O68" s="14"/>
@@ -4702,14 +4705,14 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B69" t="s">
         <v>67</v>
       </c>
       <c r="D69"/>
       <c r="F69" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>8</v>
@@ -4725,7 +4728,7 @@
         <v>"GLC-ZZ-2", "SBL", 2, "2", "(5)"</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="N69" s="34"/>
       <c r="O69" s="14"/>
@@ -4736,14 +4739,14 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B70" t="s">
         <v>67</v>
       </c>
       <c r="D70"/>
       <c r="F70" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>8</v>
@@ -4759,7 +4762,7 @@
         <v>"GLC-ZZ-3", "SBL", 2, "3", "(5)"</v>
       </c>
       <c r="M70" s="20" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="N70" s="34"/>
       <c r="O70" s="14"/>
@@ -4770,14 +4773,14 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B71" t="s">
         <v>67</v>
       </c>
       <c r="D71"/>
       <c r="F71" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>8</v>
@@ -4793,7 +4796,7 @@
         <v>"GLC-ZZ-4", "SBL", 2, "4", "(5)"</v>
       </c>
       <c r="M71" s="20" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="N71" s="34"/>
       <c r="O71" s="14"/>
@@ -4804,14 +4807,14 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
       </c>
       <c r="D72"/>
       <c r="F72" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>8</v>
@@ -4827,7 +4830,7 @@
         <v>"GLC-ZZ-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
       </c>
       <c r="M72" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="N72" s="34"/>
       <c r="O72" s="14"/>
@@ -4838,13 +4841,13 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D73">
         <v>3</v>
@@ -4857,7 +4860,7 @@
         <v>"GLC", "ST", 3, "(1)"</v>
       </c>
       <c r="M73" s="20" t="s">
-        <v>468</v>
+        <v>505</v>
       </c>
       <c r="N73" s="34"/>
       <c r="O73" s="14"/>
@@ -4868,13 +4871,13 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D74">
         <v>4</v>
@@ -4887,7 +4890,7 @@
         <v>"GLC", "ST", 4, "(1)"</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="N74" s="34"/>
       <c r="O74" s="14"/>
@@ -4898,13 +4901,13 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B75" t="s">
         <v>20</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D75">
         <v>5</v>
@@ -4917,7 +4920,7 @@
         <v>"GLC", "ST", 5, "(2)"</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>470</v>
+        <v>507</v>
       </c>
       <c r="N75" s="34"/>
       <c r="O75" s="14"/>
@@ -4928,13 +4931,13 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D76">
         <v>6</v>
@@ -4947,7 +4950,7 @@
         <v>"GLC", "ST", 6, "(2)"</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>471</v>
+        <v>508</v>
       </c>
       <c r="N76" s="34"/>
       <c r="O76" s="14"/>
@@ -4958,13 +4961,13 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B77" t="s">
         <v>20</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D77">
         <v>7</v>
@@ -4977,7 +4980,7 @@
         <v>"GLC", "ST", 7, "(3)"</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>472</v>
+        <v>509</v>
       </c>
       <c r="N77" s="34"/>
       <c r="O77" s="14"/>
@@ -4988,13 +4991,13 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B78" t="s">
         <v>20</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D78">
         <v>8</v>
@@ -5007,7 +5010,7 @@
         <v>"GLC", "ST", 8, "(3)"</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>473</v>
+        <v>510</v>
       </c>
       <c r="N78" s="34"/>
       <c r="O78" s="14"/>
@@ -5018,13 +5021,13 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B79" t="s">
         <v>20</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D79">
         <v>9</v>
@@ -5037,7 +5040,7 @@
         <v>"GLC", "ST", 9, "(4)"</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>474</v>
+        <v>511</v>
       </c>
       <c r="N79" s="34">
         <v>137</v>
@@ -5050,13 +5053,13 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D80">
         <v>11</v>
@@ -5069,7 +5072,7 @@
         <v>"GLC", "ST", 11, "(4)"</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>475</v>
+        <v>512</v>
       </c>
       <c r="N80" s="34">
         <v>137</v>
@@ -5081,34 +5084,11 @@
       <c r="S80" s="12"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>210</v>
-      </c>
-      <c r="B81" t="s">
-        <v>202</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L81" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KO-Bugla-Bry-1", "Sem(ST)+SBL", 1, "1", "(2)"</v>
-      </c>
+      <c r="D81"/>
       <c r="M81" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="N81" s="33" t="s">
-        <v>338</v>
-      </c>
+        <v>516</v>
+      </c>
+      <c r="N81" s="34"/>
       <c r="O81" s="14"/>
       <c r="P81" s="14"/>
       <c r="Q81" s="12"/>
@@ -5117,32 +5097,32 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L82" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-Bugla-Bry-2", "SBL+Sem(PODG)", 1, "2", "(2)"</v>
+        <v>"KO-Bugla-Bry-1", "Sem(ST)+SBL", 1, "1", "(2)"</v>
       </c>
       <c r="M82" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N82" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O82" s="14"/>
       <c r="P82" s="14"/>
@@ -5152,32 +5132,32 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>312</v>
+        <v>211</v>
       </c>
       <c r="B83" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>312</v>
+        <v>221</v>
       </c>
       <c r="G83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H83" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="I83" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L83" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry", "PODG", 2, "1", "(1)"</v>
+        <v>"KO-Bugla-Bry-2", "SBL+Sem(PODG)", 1, "2", "(2)"</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="N83" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O83" s="14"/>
       <c r="P83" s="14"/>
@@ -5196,7 +5176,7 @@
         <v>312</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>7</v>
@@ -5206,13 +5186,13 @@
       </c>
       <c r="L84" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry", "PODG", 1, "1", "(1)"</v>
+        <v>"Bry", "PODG", 2, "1", "(1)"</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="N84" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O84" s="14"/>
       <c r="P84" s="14"/>
@@ -5222,16 +5202,16 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="B85" t="s">
-        <v>304</v>
+        <v>46</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>110</v>
+        <v>312</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>7</v>
@@ -5241,13 +5221,13 @@
       </c>
       <c r="L85" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KO", "PODG+Sem(ST)", 2, "1", "(1)"</v>
+        <v>"Bry", "PODG", 1, "1", "(1)"</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="N85" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O85" s="14"/>
       <c r="P85" s="14"/>
@@ -5257,16 +5237,16 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>7</v>
@@ -5276,13 +5256,13 @@
       </c>
       <c r="L86" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-Bry", "ST+Sem(PODG)", 3, "1", "(1)"</v>
+        <v>"Bry-KO", "PODG+Sem(ST)", 2, "1", "(1)"</v>
       </c>
       <c r="M86" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N86" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O86" s="14"/>
       <c r="P86" s="14"/>
@@ -5292,32 +5272,32 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>313</v>
       </c>
       <c r="B87" t="s">
-        <v>68</v>
+        <v>305</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>222</v>
+        <v>109</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L87" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KL-1", "SBL+POGP", 1, "1", "(2)"</v>
+        <v>"KO-Bry", "ST+Sem(PODG)", 3, "1", "(1)"</v>
       </c>
       <c r="M87" s="20" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="N87" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O87" s="14"/>
       <c r="P87" s="14"/>
@@ -5327,32 +5307,32 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L88" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KL-2", "SBL+Sem(ST)", 1, "2", "(2)"</v>
+        <v>"Bry-KL-1", "SBL+POGP", 1, "1", "(2)"</v>
       </c>
       <c r="M88" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N88" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O88" s="14"/>
       <c r="P88" s="14"/>
@@ -5362,32 +5342,32 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B89" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L89" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-Bry-1", "SBL", 2, "1", "(2)"</v>
+        <v>"Bry-KL-2", "SBL+Sem(ST)", 1, "2", "(2)"</v>
       </c>
       <c r="M89" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N89" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O89" s="14"/>
       <c r="P89" s="14"/>
@@ -5397,32 +5377,32 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L90" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-Bry-2", "SBL+Sem(PODG)", 2, "2", "(2)"</v>
+        <v>"KL-Bry-1", "SBL", 2, "1", "(2)"</v>
       </c>
       <c r="M90" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N90" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O90" s="14"/>
       <c r="P90" s="14"/>
@@ -5432,29 +5412,32 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E91" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L91" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 1, "(2)"</v>
+        <v>"KL-Bry-2", "SBL+Sem(PODG)", 2, "2", "(2)"</v>
       </c>
       <c r="M91" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N91" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O91" s="14"/>
       <c r="P91" s="14"/>
@@ -5473,20 +5456,20 @@
         <v>112</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L92" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 2, "(2)"</v>
+        <v>"KL", "ST", 1, "(2)"</v>
       </c>
       <c r="M92" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N92" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O92" s="14"/>
       <c r="P92" s="14"/>
@@ -5505,20 +5488,20 @@
         <v>112</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L93" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 3, "(1)"</v>
+        <v>"KL", "ST", 2, "(2)"</v>
       </c>
       <c r="M93" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N93" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O93" s="14"/>
       <c r="P93" s="14"/>
@@ -5528,32 +5511,29 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
       <c r="B94" t="s">
-        <v>417</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G94" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="L94" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-MJ-1", "Sem(odstep)+PO(Piotrowice)", 1, "1", "(2)"</v>
+        <v>"KL", "ST", 3, "(1)"</v>
       </c>
       <c r="M94" s="20" t="s">
-        <v>476</v>
+        <v>289</v>
       </c>
       <c r="N94" s="33" t="s">
-        <v>404</v>
+        <v>337</v>
       </c>
       <c r="O94" s="14"/>
       <c r="P94" s="14"/>
@@ -5563,32 +5543,32 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B95" t="s">
+        <v>416</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L95" s="11" t="str">
-        <f t="shared" ref="L95:L121" si="2">IF(C95="",CONCATENATE($F$1,F95,$F$1,$G$1,$F$1,B95,$F$1,$G$1,G95,$G$1,$F$1,H95,$F$1,$G$1,$F$1,$B$1,I95,$C$1,$F$1),CONCATENATE($F$1,C95,$F$1,$G$1, $F$1,B95,$F$1,$G$1,D95,$G$1,$F$1,$B$1,E95,$C$1,$F$1))</f>
-        <v>"KL-MJ-2", "Sem(odstep)", 1, "2", "(2)"</v>
+        <f t="shared" si="1"/>
+        <v>"KL-MJ-1", "Sem(odstep)+PO(Piotrowice)", 1, "1", "(2)"</v>
       </c>
       <c r="M95" s="20" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="N95" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O95" s="14"/>
       <c r="P95" s="14"/>
@@ -5598,29 +5578,32 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D96" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G96" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>7</v>
+      <c r="H96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L96" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"MJ", "ST", 1, "(1)"</v>
+        <f t="shared" ref="L96:L122" si="2">IF(C96="",CONCATENATE($F$1,F96,$F$1,$G$1,$F$1,B96,$F$1,$G$1,G96,$G$1,$F$1,H96,$F$1,$G$1,$F$1,$B$1,I96,$C$1,$F$1),CONCATENATE($F$1,C96,$F$1,$G$1, $F$1,B96,$F$1,$G$1,D96,$G$1,$F$1,$B$1,E96,$C$1,$F$1))</f>
+        <v>"KL-MJ-2", "Sem(odstep)", 1, "2", "(2)"</v>
       </c>
       <c r="M96" s="20" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="N96" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O96" s="14"/>
       <c r="P96" s="14"/>
@@ -5630,29 +5613,29 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L97" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"MJ", "ST", 2, "(1)"</v>
+        <v>"MJ", "ST", 1, "(1)"</v>
       </c>
       <c r="M97" s="20" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="N97" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O97" s="14"/>
       <c r="P97" s="14"/>
@@ -5662,32 +5645,29 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B98" t="s">
-        <v>373</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I98" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L98" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"MJ-Mi", "Sem(odstep)", 1, "1", "(1)"</v>
+        <v>"MJ", "ST", 2, "(1)"</v>
       </c>
       <c r="M98" s="20" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="N98" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O98" s="14"/>
       <c r="P98" s="14"/>
@@ -5697,29 +5677,32 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D99" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="H99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L99" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mi", "ST", 1, "(1)"</v>
+        <v>"MJ-Mi", "Sem(odstep)", 1, "1", "(1)"</v>
       </c>
       <c r="M99" s="20" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="N99" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O99" s="14"/>
       <c r="P99" s="14"/>
@@ -5729,29 +5712,29 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L100" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mi", "ST", 2, "(1)"</v>
+        <v>"Mi", "ST", 1, "(1)"</v>
       </c>
       <c r="M100" s="20" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="N100" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O100" s="14"/>
       <c r="P100" s="14"/>
@@ -5761,32 +5744,29 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B101" t="s">
-        <v>418</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="G101" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="L101" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
+        <v>"Mi", "ST", 2, "(1)"</v>
       </c>
       <c r="M101" s="20" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="N101" s="33" t="s">
-        <v>338</v>
+        <v>403</v>
       </c>
       <c r="O101" s="14"/>
       <c r="P101" s="14"/>
@@ -5796,32 +5776,32 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B102" t="s">
-        <v>67</v>
+        <v>417</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L102" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
+        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
       </c>
       <c r="M102" s="20" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="N102" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O102" s="14"/>
       <c r="P102" s="14"/>
@@ -5831,32 +5811,32 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B103" t="s">
         <v>67</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L103" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
+        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
       </c>
       <c r="M103" s="20" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="N103" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O103" s="14"/>
       <c r="P103" s="14"/>
@@ -5866,32 +5846,32 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B104" t="s">
-        <v>419</v>
+        <v>67</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L104" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
+        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="N104" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O104" s="14"/>
       <c r="P104" s="14"/>
@@ -5901,32 +5881,32 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>418</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L105" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
+        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
       </c>
       <c r="M105" s="20" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="N105" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O105" s="14"/>
       <c r="P105" s="14"/>
@@ -5936,32 +5916,32 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>420</v>
+        <v>113</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L106" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
+        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="N106" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O106" s="14"/>
       <c r="P106" s="14"/>
@@ -5971,32 +5951,32 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>500</v>
+        <v>425</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L107" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
+        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>505</v>
+        <v>477</v>
       </c>
       <c r="N107" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O107" s="14"/>
       <c r="P107" s="14"/>
@@ -6006,32 +5986,32 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B108" t="s">
-        <v>419</v>
+        <v>67</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L108" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
+        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="N108" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O108" s="14"/>
       <c r="P108" s="14"/>
@@ -6041,32 +6021,32 @@
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B109" t="s">
-        <v>67</v>
+        <v>418</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L109" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
+        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="N109" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O109" s="14"/>
       <c r="P109" s="14"/>
@@ -6076,32 +6056,32 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B110" t="s">
         <v>67</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L110" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
+        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
       <c r="N110" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O110" s="14"/>
       <c r="P110" s="14"/>
@@ -6111,32 +6091,32 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B111" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L111" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
+        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="N111" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O111" s="14"/>
       <c r="P111" s="14"/>
@@ -6146,29 +6126,32 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="B112" t="s">
-        <v>46</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>105</v>
+        <v>77</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L112" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 1, "(N/A)"</v>
+        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
       <c r="N112" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O112" s="14"/>
       <c r="P112" s="14"/>
@@ -6178,26 +6161,29 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B113" t="s">
         <v>46</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L113" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 2, "(N/A)"</v>
+        <v>"Mc", "PODG", 1, "(N/A)"</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>490</v>
+        <v>478</v>
+      </c>
+      <c r="N113" s="33" t="s">
+        <v>337</v>
       </c>
       <c r="O113" s="14"/>
       <c r="P113" s="14"/>
@@ -6207,26 +6193,26 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B114" t="s">
         <v>46</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L114" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 3, "(N/A)"</v>
+        <v>"Mc", "PODG", 2, "(N/A)"</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="O114" s="14"/>
       <c r="P114" s="14"/>
@@ -6236,32 +6222,26 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>439</v>
+        <v>404</v>
       </c>
       <c r="B115" t="s">
-        <v>427</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="L115" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
+        <v>"Mc", "PODG", 3, "(N/A)"</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>492</v>
-      </c>
-      <c r="N115" s="33" t="s">
-        <v>338</v>
+        <v>480</v>
       </c>
       <c r="O115" s="14"/>
       <c r="P115" s="14"/>
@@ -6274,13 +6254,13 @@
         <v>438</v>
       </c>
       <c r="B116" t="s">
-        <v>373</v>
+        <v>426</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>7</v>
@@ -6290,13 +6270,13 @@
       </c>
       <c r="L116" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
+        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="N116" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O116" s="14"/>
       <c r="P116" s="14"/>
@@ -6309,13 +6289,13 @@
         <v>437</v>
       </c>
       <c r="B117" t="s">
-        <v>434</v>
+        <v>372</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>7</v>
@@ -6325,13 +6305,13 @@
       </c>
       <c r="L117" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
+        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="N117" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O117" s="14"/>
       <c r="P117" s="14"/>
@@ -6341,29 +6321,32 @@
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="B118" t="s">
-        <v>20</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>105</v>
+        <v>433</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L118" s="11" t="str">
-        <f t="shared" ref="L118:L120" si="3">IF(C118="",CONCATENATE($F$1,F118,$F$1,$G$1,$F$1,B118,$F$1,$G$1,G118,$G$1,$F$1,H118,$F$1,$G$1,$F$1,$B$1,I118,$C$1,$F$1),CONCATENATE($F$1,C118,$F$1,$G$1, $F$1,B118,$F$1,$G$1,D118,$G$1,$F$1,$B$1,E118,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 101, "(N/A)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="N118" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O118" s="14"/>
       <c r="P118" s="14"/>
@@ -6373,29 +6356,29 @@
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B119" t="s">
         <v>20</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L119" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>"Ty", "ST", 102, "(N/A)"</v>
+        <f t="shared" ref="L119:L121" si="3">IF(C119="",CONCATENATE($F$1,F119,$F$1,$G$1,$F$1,B119,$F$1,$G$1,G119,$G$1,$F$1,H119,$F$1,$G$1,$F$1,$B$1,I119,$C$1,$F$1),CONCATENATE($F$1,C119,$F$1,$G$1, $F$1,B119,$F$1,$G$1,D119,$G$1,$F$1,$B$1,E119,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 101, "(N/A)"</v>
       </c>
       <c r="M119" s="20" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="N119" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O119" s="14"/>
       <c r="P119" s="14"/>
@@ -6405,29 +6388,29 @@
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B120" t="s">
         <v>20</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L120" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>"Ty", "ST", 108, "(N/A)"</v>
+        <v>"Ty", "ST", 102, "(N/A)"</v>
       </c>
       <c r="M120" s="20" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="N120" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O120" s="14"/>
       <c r="P120" s="14"/>
@@ -6437,29 +6420,29 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B121" t="s">
         <v>20</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>7</v>
+        <v>501</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="L121" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"Ty", "ST", 1, "(2)"</v>
+        <f t="shared" si="3"/>
+        <v>"Ty", "ST", 108, "(N/A)"</v>
       </c>
       <c r="M121" s="20" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="N121" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O121" s="14"/>
       <c r="P121" s="14"/>
@@ -6469,29 +6452,29 @@
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B122" t="s">
         <v>20</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L122" s="11" t="str">
-        <f t="shared" ref="L122:L125" si="4">IF(C122="",CONCATENATE($F$1,F122,$F$1,$G$1,$F$1,B122,$F$1,$G$1,G122,$G$1,$F$1,H122,$F$1,$G$1,$F$1,$B$1,I122,$C$1,$F$1),CONCATENATE($F$1,C122,$F$1,$G$1, $F$1,B122,$F$1,$G$1,D122,$G$1,$F$1,$B$1,E122,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 2, "(2)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty", "ST", 1, "(2)"</v>
       </c>
       <c r="M122" s="20" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="N122" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O122" s="14"/>
       <c r="P122" s="14"/>
@@ -6501,29 +6484,29 @@
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>431</v>
+        <v>8</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L123" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>"Ty", "ST", 8, "(1)"</v>
+        <f t="shared" ref="L123:L126" si="4">IF(C123="",CONCATENATE($F$1,F123,$F$1,$G$1,$F$1,B123,$F$1,$G$1,G123,$G$1,$F$1,H123,$F$1,$G$1,$F$1,$B$1,I123,$C$1,$F$1),CONCATENATE($F$1,C123,$F$1,$G$1, $F$1,B123,$F$1,$G$1,D123,$G$1,$F$1,$B$1,E123,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 2, "(2)"</v>
       </c>
       <c r="M123" s="20" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="N123" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O123" s="14"/>
       <c r="P123" s="14"/>
@@ -6533,29 +6516,29 @@
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L124" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>"Ty", "ST", 7, "(3)"</v>
+        <v>"Ty", "ST", 8, "(1)"</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="N124" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O124" s="14"/>
       <c r="P124" s="14"/>
@@ -6565,29 +6548,29 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L125" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>"Ty", "ST", 9, "(3)"</v>
+        <v>"Ty", "ST", 7, "(3)"</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="N125" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O125" s="14"/>
       <c r="P125" s="14"/>
@@ -6597,32 +6580,29 @@
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>116</v>
+        <v>429</v>
       </c>
       <c r="B126" t="s">
-        <v>77</v>
-      </c>
-      <c r="F126" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G126" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I126" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L126" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty", "ST", 9, "(3)"</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>290</v>
+        <v>488</v>
       </c>
       <c r="N126" s="33" t="s">
-        <v>7</v>
+        <v>337</v>
       </c>
       <c r="O126" s="14"/>
       <c r="P126" s="14"/>
@@ -6632,16 +6612,16 @@
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B127" t="s">
         <v>77</v>
       </c>
       <c r="F127" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>7</v>
@@ -6651,10 +6631,10 @@
       </c>
       <c r="L127" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N127" s="33" t="s">
         <v>7</v>
@@ -6667,16 +6647,16 @@
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B128" t="s">
         <v>77</v>
       </c>
       <c r="F128" s="31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>7</v>
@@ -6686,13 +6666,13 @@
       </c>
       <c r="L128" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
+        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
       </c>
       <c r="M128" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N128" s="33" t="s">
-        <v>339</v>
+        <v>7</v>
       </c>
       <c r="O128" s="14"/>
       <c r="P128" s="14"/>
@@ -6702,16 +6682,16 @@
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B129" t="s">
         <v>77</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H129" s="2" t="s">
         <v>7</v>
@@ -6721,13 +6701,13 @@
       </c>
       <c r="L129" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
       </c>
       <c r="M129" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N129" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O129" s="14"/>
       <c r="P129" s="14"/>
@@ -6737,29 +6717,32 @@
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
-      </c>
-      <c r="C130" t="s">
-        <v>144</v>
-      </c>
-      <c r="D130" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F130" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H130" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="I130" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L130" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 1, "(1)"</v>
+        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
       </c>
       <c r="M130" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N130" s="33" t="s">
-        <v>7</v>
+        <v>338</v>
       </c>
       <c r="O130" s="14"/>
       <c r="P130" s="14"/>
@@ -6778,17 +6761,17 @@
         <v>144</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L131" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 2, "(1)"</v>
+        <v>"KZ", "ST", 1, "(1)"</v>
       </c>
       <c r="M131" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N131" s="33" t="s">
         <v>7</v>
@@ -6810,20 +6793,20 @@
         <v>144</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L132" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 3, "(2)"</v>
+        <v>"KZ", "ST", 2, "(1)"</v>
       </c>
       <c r="M132" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N132" s="33" t="s">
-        <v>339</v>
+        <v>7</v>
       </c>
       <c r="O132" s="14"/>
       <c r="P132" s="14"/>
@@ -6842,20 +6825,20 @@
         <v>144</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L133" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 4, "(2)"</v>
+        <v>"KZ", "ST", 3, "(2)"</v>
       </c>
       <c r="M133" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N133" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O133" s="14"/>
       <c r="P133" s="14"/>
@@ -6864,12 +6847,30 @@
       <c r="S133" s="12"/>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>143</v>
+      </c>
+      <c r="B134" t="s">
+        <v>20</v>
+      </c>
+      <c r="C134" t="s">
+        <v>144</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L134" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"", "", , "", "()"</v>
+        <v>"KZ", "ST", 4, "(2)"</v>
       </c>
       <c r="M134" s="20" t="s">
-        <v>184</v>
+        <v>297</v>
+      </c>
+      <c r="N134" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O134" s="14"/>
       <c r="P134" s="14"/>
@@ -6879,7 +6880,7 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L135" s="11" t="str">
-        <f t="shared" ref="L135:L198" si="5">IF(C135="",CONCATENATE($F$1,F135,$F$1,$G$1,$F$1,B135,$F$1,$G$1,G135,$G$1,$F$1,H135,$F$1,$G$1,$F$1,$B$1,I135,$C$1,$F$1),CONCATENATE($F$1,C135,$F$1,$G$1, $F$1,B135,$F$1,$G$1,D135,$G$1,$F$1,$B$1,E135,$C$1,$F$1))</f>
+        <f t="shared" si="1"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M135" s="20" t="s">
@@ -6893,7 +6894,7 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L136" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="L136:L199" si="5">IF(C136="",CONCATENATE($F$1,F136,$F$1,$G$1,$F$1,B136,$F$1,$G$1,G136,$G$1,$F$1,H136,$F$1,$G$1,$F$1,$B$1,I136,$C$1,$F$1),CONCATENATE($F$1,C136,$F$1,$G$1, $F$1,B136,$F$1,$G$1,D136,$G$1,$F$1,$B$1,E136,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M136" s="20" t="s">
@@ -7067,6 +7068,11 @@
       <c r="M148" s="20" t="s">
         <v>184</v>
       </c>
+      <c r="O148" s="14"/>
+      <c r="P148" s="14"/>
+      <c r="Q148" s="12"/>
+      <c r="R148" s="12"/>
+      <c r="S148" s="12"/>
     </row>
     <row r="149" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L149" s="11" t="str">
@@ -7520,7 +7526,7 @@
     </row>
     <row r="199" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L199" s="11" t="str">
-        <f t="shared" ref="L199:L262" si="6">IF(C199="",CONCATENATE($F$1,F199,$F$1,$G$1,$F$1,B199,$F$1,$G$1,G199,$G$1,$F$1,H199,$F$1,$G$1,$F$1,$B$1,I199,$C$1,$F$1),CONCATENATE($F$1,C199,$F$1,$G$1, $F$1,B199,$F$1,$G$1,D199,$G$1,$F$1,$B$1,E199,$C$1,$F$1))</f>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M199" s="20" t="s">
@@ -7529,7 +7535,7 @@
     </row>
     <row r="200" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L200" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="L200:L263" si="6">IF(C200="",CONCATENATE($F$1,F200,$F$1,$G$1,$F$1,B200,$F$1,$G$1,G200,$G$1,$F$1,H200,$F$1,$G$1,$F$1,$B$1,I200,$C$1,$F$1),CONCATENATE($F$1,C200,$F$1,$G$1, $F$1,B200,$F$1,$G$1,D200,$G$1,$F$1,$B$1,E200,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M200" s="20" t="s">
@@ -8096,7 +8102,7 @@
     </row>
     <row r="263" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L263" s="11" t="str">
-        <f t="shared" ref="L263:L326" si="7">IF(C263="",CONCATENATE($F$1,F263,$F$1,$G$1,$F$1,B263,$F$1,$G$1,G263,$G$1,$F$1,H263,$F$1,$G$1,$F$1,$B$1,I263,$C$1,$F$1),CONCATENATE($F$1,C263,$F$1,$G$1, $F$1,B263,$F$1,$G$1,D263,$G$1,$F$1,$B$1,E263,$C$1,$F$1))</f>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M263" s="20" t="s">
@@ -8105,7 +8111,7 @@
     </row>
     <row r="264" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L264" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L264:L327" si="7">IF(C264="",CONCATENATE($F$1,F264,$F$1,$G$1,$F$1,B264,$F$1,$G$1,G264,$G$1,$F$1,H264,$F$1,$G$1,$F$1,$B$1,I264,$C$1,$F$1),CONCATENATE($F$1,C264,$F$1,$G$1, $F$1,B264,$F$1,$G$1,D264,$G$1,$F$1,$B$1,E264,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M264" s="20" t="s">
@@ -8672,7 +8678,7 @@
     </row>
     <row r="327" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L327" s="11" t="str">
-        <f t="shared" ref="L327:L390" si="8">IF(C327="",CONCATENATE($F$1,F327,$F$1,$G$1,$F$1,B327,$F$1,$G$1,G327,$G$1,$F$1,H327,$F$1,$G$1,$F$1,$B$1,I327,$C$1,$F$1),CONCATENATE($F$1,C327,$F$1,$G$1, $F$1,B327,$F$1,$G$1,D327,$G$1,$F$1,$B$1,E327,$C$1,$F$1))</f>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M327" s="20" t="s">
@@ -8681,7 +8687,7 @@
     </row>
     <row r="328" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L328" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L328:L391" si="8">IF(C328="",CONCATENATE($F$1,F328,$F$1,$G$1,$F$1,B328,$F$1,$G$1,G328,$G$1,$F$1,H328,$F$1,$G$1,$F$1,$B$1,I328,$C$1,$F$1),CONCATENATE($F$1,C328,$F$1,$G$1, $F$1,B328,$F$1,$G$1,D328,$G$1,$F$1,$B$1,E328,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M328" s="20" t="s">
@@ -9248,7 +9254,7 @@
     </row>
     <row r="391" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L391" s="11" t="str">
-        <f t="shared" ref="L391:L399" si="9">IF(C391="",CONCATENATE($F$1,F391,$F$1,$G$1,$F$1,B391,$F$1,$G$1,G391,$G$1,$F$1,H391,$F$1,$G$1,$F$1,$B$1,I391,$C$1,$F$1),CONCATENATE($F$1,C391,$F$1,$G$1, $F$1,B391,$F$1,$G$1,D391,$G$1,$F$1,$B$1,E391,$C$1,$F$1))</f>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M391" s="20" t="s">
@@ -9257,7 +9263,7 @@
     </row>
     <row r="392" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L392" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="L392:L400" si="9">IF(C392="",CONCATENATE($F$1,F392,$F$1,$G$1,$F$1,B392,$F$1,$G$1,G392,$G$1,$F$1,H392,$F$1,$G$1,$F$1,$B$1,I392,$C$1,$F$1),CONCATENATE($F$1,C392,$F$1,$G$1, $F$1,B392,$F$1,$G$1,D392,$G$1,$F$1,$B$1,E392,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M392" s="20" t="s">
@@ -9324,6 +9330,15 @@
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M399" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="400" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L400" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M400" s="20" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates in train paths
</commit_message>
<xml_diff>
--- a/data/Spis odcinków_KO-CB-KZ-KL.xlsx
+++ b/data/Spis odcinków_KO-CB-KZ-KL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\railways_dispatching_silesia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6E5DBA-3A0F-455B-856F-4084B54F9D45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADCE2CA-8EEA-457B-9A50-D8AD2AB9B8A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="538">
   <si>
     <t>Katowice</t>
   </si>
@@ -1434,15 +1434,9 @@
     <t>"MJ", "ST", 1, "(1)"</t>
   </si>
   <si>
-    <t>"MJ", "ST", 2, "(1)"</t>
-  </si>
-  <si>
     <t>"MJ-Mi", "Sem(odstep)", 1, "1", "(1)"</t>
   </si>
   <si>
-    <t>"Mi", "ST", 1, "(1)"</t>
-  </si>
-  <si>
     <t>"Mi", "ST", 2, "(1)"</t>
   </si>
   <si>
@@ -1579,6 +1573,75 @@
   </si>
   <si>
     <t>"GLC(KS)", "B-M", 200, "(N/A)"</t>
+  </si>
+  <si>
+    <t>"MJ", "ST", 3, "(2)"</t>
+  </si>
+  <si>
+    <t>"Mi", "ST", 1, "(2)"</t>
+  </si>
+  <si>
+    <t>GLC(KS)</t>
+  </si>
+  <si>
+    <t>GLC-Szo</t>
+  </si>
+  <si>
+    <t>Szo-GLC</t>
+  </si>
+  <si>
+    <t>SBL(odstep)</t>
+  </si>
+  <si>
+    <t>"GLC-Szo", "Sem(odstep)", 1, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"Szo-GLC", "SBL(odstep)", 2, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>KZ-Szb</t>
+  </si>
+  <si>
+    <t>Szb-KZ</t>
+  </si>
+  <si>
+    <t>KZ-Szb_1</t>
+  </si>
+  <si>
+    <t>Szb-KZ_3</t>
+  </si>
+  <si>
+    <t>KZ-SG</t>
+  </si>
+  <si>
+    <t>SG-KZ</t>
+  </si>
+  <si>
+    <t>"KZ-SG", "", 1, "1", "(3)"</t>
+  </si>
+  <si>
+    <t>"SG-KZ", "", 2, "3", "(3)"</t>
+  </si>
+  <si>
+    <t>"KZ-Szb_1", "SBL", 3, "2", "(2)"</t>
+  </si>
+  <si>
+    <t>"Szb-KZ_3", "SBL+Sem(ST)", 4, "1", "(3)"</t>
+  </si>
+  <si>
+    <t>CM-CS</t>
+  </si>
+  <si>
+    <t>CS-CM</t>
+  </si>
+  <si>
+    <t>Sem(odstęp)</t>
+  </si>
+  <si>
+    <t>"CM-CS", "Sem(odstęp)", 1, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"CS-CM", "Sem(odstęp)", 2, "1", "(1)"</t>
   </si>
 </sst>
 </file>
@@ -2156,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM400"/>
+  <dimension ref="A1:AM404"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M81" sqref="M81"/>
+      <selection activeCell="M84" sqref="M84:M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2230,9 @@
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="9.5703125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="19" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="37.28515625" style="11" customWidth="1"/>
@@ -3044,7 +3109,7 @@
       </c>
       <c r="F23" s="17"/>
       <c r="L23" s="11" t="str">
-        <f t="shared" ref="L23:L135" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
+        <f t="shared" ref="L23:L139" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
         <v>"KO", "ST-M", 1114, "(N/A)"</v>
       </c>
       <c r="M23" s="11" t="s">
@@ -3788,7 +3853,7 @@
         <v>"CM-CB", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N42" s="33" t="s">
         <v>336</v>
@@ -3865,14 +3930,14 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>340</v>
+        <v>533</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>535</v>
       </c>
       <c r="D45"/>
       <c r="F45" s="2" t="s">
-        <v>375</v>
+        <v>533</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>7</v>
@@ -3881,17 +3946,14 @@
         <v>7</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L45" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"CB-RCB-1", "SBL", 1, "1", "(3)"</v>
+        <v>"CM-CS", "Sem(odstęp)", 1, "1", "(1)"</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>439</v>
-      </c>
-      <c r="N45" s="34">
-        <v>137</v>
+        <v>536</v>
       </c>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
@@ -3901,33 +3963,30 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>339</v>
+        <v>534</v>
       </c>
       <c r="B46" t="s">
-        <v>345</v>
+        <v>535</v>
       </c>
       <c r="D46"/>
       <c r="F46" s="2" t="s">
-        <v>376</v>
+        <v>534</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I46" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L46" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"CB-RCB-2", "SBL+PO(Świętochłowice)", 1, "2", "(3)"</v>
+        <v>"CS-CM", "Sem(odstęp)", 2, "1", "(1)"</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="N46" s="34">
-        <v>137</v>
+        <v>537</v>
       </c>
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
@@ -3937,30 +3996,30 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D47"/>
       <c r="F47" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L47" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"CB-RCB-3", "SBL+Sem(ST)", 1, "3", "(3)"</v>
+        <v>"CB-RCB-1", "SBL", 1, "1", "(3)"</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="N47" s="34">
         <v>137</v>
@@ -3973,30 +4032,30 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>345</v>
       </c>
       <c r="D48"/>
       <c r="F48" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L48" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-CB-1", "SBL", 2, "1", "(3)"</v>
+        <v>"CB-RCB-2", "SBL+PO(Świętochłowice)", 1, "2", "(3)"</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N48" s="34">
         <v>137</v>
@@ -4009,30 +4068,30 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>345</v>
+        <v>77</v>
       </c>
       <c r="D49"/>
       <c r="F49" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L49" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-CB-2", "SBL+PO(Świętochłowice)", 2, "2", "(3)"</v>
+        <v>"CB-RCB-3", "SBL+Sem(ST)", 1, "3", "(3)"</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="N49" s="34">
         <v>137</v>
@@ -4045,30 +4104,30 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D50"/>
       <c r="F50" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L50" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-CB-3", "SBL+Sem(ST)", 2, "3", "(3)"</v>
+        <v>"RCB-CB-1", "SBL", 2, "1", "(3)"</v>
       </c>
       <c r="M50" s="20" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="N50" s="34">
         <v>137</v>
@@ -4081,26 +4140,30 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>7</v>
+        <v>345</v>
+      </c>
+      <c r="D51"/>
+      <c r="F51" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L51" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB", "ST", 1, "(1)"</v>
+        <v>"RCB-CB-2", "SBL+PO(Świętochłowice)", 2, "2", "(3)"</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="N51" s="34">
         <v>137</v>
@@ -4113,26 +4176,30 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
+      </c>
+      <c r="D52"/>
+      <c r="F52" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L52" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB", "ST", 2, "(1)"</v>
+        <v>"RCB-CB-3", "SBL+Sem(ST)", 2, "3", "(3)"</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="N52" s="34">
         <v>137</v>
@@ -4145,30 +4212,26 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53"/>
-      <c r="F53" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="G53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="L53" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-ZZ-1", "SBL", 1, "1", "(4)"</v>
+        <v>"RCB", "ST", 1, "(1)"</v>
       </c>
       <c r="M53" s="20" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="N53" s="34">
         <v>137</v>
@@ -4181,30 +4244,26 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B54" t="s">
-        <v>345</v>
-      </c>
-      <c r="D54"/>
-      <c r="F54" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="G54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="L54" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</v>
+        <v>"RCB", "ST", 2, "(1)"</v>
       </c>
       <c r="M54" s="20" t="s">
-        <v>514</v>
+        <v>446</v>
       </c>
       <c r="N54" s="34">
         <v>137</v>
@@ -4217,30 +4276,30 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B55" t="s">
         <v>67</v>
       </c>
       <c r="D55"/>
       <c r="F55" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L55" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-ZZ-3", "SBL", 1, "3", "(4)"</v>
+        <v>"RCB-ZZ-1", "SBL", 1, "1", "(4)"</v>
       </c>
       <c r="M55" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="N55" s="34">
         <v>137</v>
@@ -4253,30 +4312,30 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>345</v>
       </c>
       <c r="D56"/>
       <c r="F56" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L56" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"RCB-ZZ-4", "SBL+Sem(ST)", 1, "4", "(4)"</v>
+        <v>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>449</v>
+        <v>512</v>
       </c>
       <c r="N56" s="34">
         <v>137</v>
@@ -4289,30 +4348,30 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B57" t="s">
         <v>67</v>
       </c>
       <c r="D57"/>
       <c r="F57" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L57" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-RCB-1", "SBL", 2, "1", "(4)"</v>
+        <v>"RCB-ZZ-3", "SBL", 1, "3", "(4)"</v>
       </c>
       <c r="M57" s="20" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="N57" s="34">
         <v>137</v>
@@ -4325,30 +4384,30 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D58"/>
       <c r="F58" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L58" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-RCB-2", "SBL", 2, "2", "(4)"</v>
+        <v>"RCB-ZZ-4", "SBL+Sem(ST)", 1, "4", "(4)"</v>
       </c>
       <c r="M58" s="20" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="N58" s="34">
         <v>137</v>
@@ -4361,30 +4420,30 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B59" t="s">
-        <v>345</v>
+        <v>67</v>
       </c>
       <c r="D59"/>
       <c r="F59" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L59" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</v>
+        <v>"ZZ-RCB-1", "SBL", 2, "1", "(4)"</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>515</v>
+        <v>450</v>
       </c>
       <c r="N59" s="34">
         <v>137</v>
@@ -4397,30 +4456,30 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D60"/>
       <c r="F60" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L60" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-RCB-4", "SBL+Sem(ST)", 2, "4", "(4)"</v>
+        <v>"ZZ-RCB-2", "SBL", 2, "2", "(4)"</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N60" s="34">
         <v>137</v>
@@ -4433,26 +4492,30 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>7</v>
+        <v>345</v>
+      </c>
+      <c r="D61"/>
+      <c r="F61" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="L61" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ", "ST", 1, "(1)"</v>
+        <v>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>453</v>
+        <v>513</v>
       </c>
       <c r="N61" s="34">
         <v>137</v>
@@ -4465,26 +4528,30 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
+      </c>
+      <c r="D62"/>
+      <c r="F62" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="L62" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ", "ST", 2, "(1)"</v>
+        <v>"ZZ-RCB-4", "SBL+Sem(ST)", 2, "4", "(4)"</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="N62" s="34">
         <v>137</v>
@@ -4497,30 +4564,26 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
-      </c>
-      <c r="D63"/>
-      <c r="F63" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="G63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="L63" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-GLC-1", "SBL", 1, "1", "(5)"</v>
+        <v>"ZZ", "ST", 1, "(1)"</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="N63" s="34">
         <v>137</v>
@@ -4533,30 +4596,26 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64"/>
-      <c r="F64" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="G64" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="L64" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-GLC-2", "SBL", 1, "2", "(5)"</v>
+        <v>"ZZ", "ST", 2, "(1)"</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="N64" s="34">
         <v>137</v>
@@ -4569,32 +4628,34 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B65" t="s">
         <v>67</v>
       </c>
       <c r="D65"/>
       <c r="F65" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L65" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-GLC-3", "SBL", 1, "3", "(5)"</v>
+        <v>"ZZ-GLC-1", "SBL", 1, "1", "(5)"</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>457</v>
-      </c>
-      <c r="N65" s="34"/>
+        <v>455</v>
+      </c>
+      <c r="N65" s="34">
+        <v>137</v>
+      </c>
       <c r="O65" s="14"/>
       <c r="P65" s="14"/>
       <c r="Q65" s="12"/>
@@ -4603,32 +4664,34 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B66" t="s">
         <v>67</v>
       </c>
       <c r="D66"/>
       <c r="F66" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L66" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-GLC-4", "SBL", 1, "4", "(5)"</v>
+        <v>"ZZ-GLC-2", "SBL", 1, "2", "(5)"</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>458</v>
-      </c>
-      <c r="N66" s="34"/>
+        <v>456</v>
+      </c>
+      <c r="N66" s="34">
+        <v>137</v>
+      </c>
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
       <c r="Q66" s="12"/>
@@ -4637,32 +4700,34 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D67"/>
       <c r="F67" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L67" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"ZZ-GLC-5", "SBL+Sem(ST)", 1, "5", "(5)"</v>
+        <v>"ZZ-GLC-3", "SBL", 1, "3", "(5)"</v>
       </c>
       <c r="M67" s="20" t="s">
-        <v>459</v>
-      </c>
-      <c r="N67" s="34"/>
+        <v>457</v>
+      </c>
+      <c r="N67" s="34">
+        <v>137</v>
+      </c>
       <c r="O67" s="14"/>
       <c r="P67" s="14"/>
       <c r="Q67" s="12"/>
@@ -4671,32 +4736,34 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
       <c r="D68"/>
       <c r="F68" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L68" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC-ZZ-1", "SBL", 2, "1", "(5)"</v>
+        <v>"ZZ-GLC-4", "SBL", 1, "4", "(5)"</v>
       </c>
       <c r="M68" s="20" t="s">
-        <v>460</v>
-      </c>
-      <c r="N68" s="34"/>
+        <v>458</v>
+      </c>
+      <c r="N68" s="34">
+        <v>137</v>
+      </c>
       <c r="O68" s="14"/>
       <c r="P68" s="14"/>
       <c r="Q68" s="12"/>
@@ -4705,32 +4772,34 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D69"/>
       <c r="F69" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L69" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC-ZZ-2", "SBL", 2, "2", "(5)"</v>
+        <v>"ZZ-GLC-5", "SBL+Sem(ST)", 1, "5", "(5)"</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="N69" s="34"/>
+        <v>459</v>
+      </c>
+      <c r="N69" s="34">
+        <v>137</v>
+      </c>
       <c r="O69" s="14"/>
       <c r="P69" s="14"/>
       <c r="Q69" s="12"/>
@@ -4739,32 +4808,34 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B70" t="s">
         <v>67</v>
       </c>
       <c r="D70"/>
       <c r="F70" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L70" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC-ZZ-3", "SBL", 2, "3", "(5)"</v>
+        <v>"GLC-ZZ-1", "SBL", 2, "1", "(5)"</v>
       </c>
       <c r="M70" s="20" t="s">
-        <v>462</v>
-      </c>
-      <c r="N70" s="34"/>
+        <v>460</v>
+      </c>
+      <c r="N70" s="34">
+        <v>137</v>
+      </c>
       <c r="O70" s="14"/>
       <c r="P70" s="14"/>
       <c r="Q70" s="12"/>
@@ -4773,32 +4844,34 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B71" t="s">
         <v>67</v>
       </c>
       <c r="D71"/>
       <c r="F71" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L71" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC-ZZ-4", "SBL", 2, "4", "(5)"</v>
+        <v>"GLC-ZZ-2", "SBL", 2, "2", "(5)"</v>
       </c>
       <c r="M71" s="20" t="s">
-        <v>463</v>
-      </c>
-      <c r="N71" s="34"/>
+        <v>461</v>
+      </c>
+      <c r="N71" s="34">
+        <v>137</v>
+      </c>
       <c r="O71" s="14"/>
       <c r="P71" s="14"/>
       <c r="Q71" s="12"/>
@@ -4807,32 +4880,34 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D72"/>
       <c r="F72" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L72" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC-ZZ-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
+        <v>"GLC-ZZ-3", "SBL", 2, "3", "(5)"</v>
       </c>
       <c r="M72" s="20" t="s">
-        <v>464</v>
-      </c>
-      <c r="N72" s="34"/>
+        <v>462</v>
+      </c>
+      <c r="N72" s="34">
+        <v>137</v>
+      </c>
       <c r="O72" s="14"/>
       <c r="P72" s="14"/>
       <c r="Q72" s="12"/>
@@ -4841,28 +4916,34 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D73">
-        <v>3</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="D73"/>
+      <c r="F73" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L73" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 3, "(1)"</v>
+        <v>"GLC-ZZ-4", "SBL", 2, "4", "(5)"</v>
       </c>
       <c r="M73" s="20" t="s">
-        <v>505</v>
-      </c>
-      <c r="N73" s="34"/>
+        <v>463</v>
+      </c>
+      <c r="N73" s="34">
+        <v>137</v>
+      </c>
       <c r="O73" s="14"/>
       <c r="P73" s="14"/>
       <c r="Q73" s="12"/>
@@ -4871,28 +4952,34 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D74">
-        <v>4</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
+      </c>
+      <c r="D74"/>
+      <c r="F74" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L74" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 4, "(1)"</v>
+        <v>"GLC-ZZ-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>506</v>
-      </c>
-      <c r="N74" s="34"/>
+        <v>464</v>
+      </c>
+      <c r="N74" s="34">
+        <v>137</v>
+      </c>
       <c r="O74" s="14"/>
       <c r="P74" s="14"/>
       <c r="Q74" s="12"/>
@@ -4910,19 +4997,21 @@
         <v>369</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L75" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 5, "(2)"</v>
+        <v>"GLC", "ST", 3, "(1)"</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="N75" s="34"/>
+        <v>503</v>
+      </c>
+      <c r="N75" s="34">
+        <v>137</v>
+      </c>
       <c r="O75" s="14"/>
       <c r="P75" s="14"/>
       <c r="Q75" s="12"/>
@@ -4940,19 +5029,21 @@
         <v>369</v>
       </c>
       <c r="D76">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L76" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 6, "(2)"</v>
+        <v>"GLC", "ST", 4, "(1)"</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>508</v>
-      </c>
-      <c r="N76" s="34"/>
+        <v>504</v>
+      </c>
+      <c r="N76" s="34">
+        <v>137</v>
+      </c>
       <c r="O76" s="14"/>
       <c r="P76" s="14"/>
       <c r="Q76" s="12"/>
@@ -4970,19 +5061,21 @@
         <v>369</v>
       </c>
       <c r="D77">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L77" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 7, "(3)"</v>
+        <v>"GLC", "ST", 5, "(2)"</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="N77" s="34"/>
+        <v>505</v>
+      </c>
+      <c r="N77" s="34">
+        <v>137</v>
+      </c>
       <c r="O77" s="14"/>
       <c r="P77" s="14"/>
       <c r="Q77" s="12"/>
@@ -5000,19 +5093,21 @@
         <v>369</v>
       </c>
       <c r="D78">
+        <v>6</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="L78" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 8, "(3)"</v>
+        <v>"GLC", "ST", 6, "(2)"</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>510</v>
-      </c>
-      <c r="N78" s="34"/>
+        <v>506</v>
+      </c>
+      <c r="N78" s="34">
+        <v>137</v>
+      </c>
       <c r="O78" s="14"/>
       <c r="P78" s="14"/>
       <c r="Q78" s="12"/>
@@ -5030,17 +5125,17 @@
         <v>369</v>
       </c>
       <c r="D79">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L79" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 9, "(4)"</v>
+        <v>"GLC", "ST", 7, "(3)"</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="N79" s="34">
         <v>137</v>
@@ -5062,17 +5157,17 @@
         <v>369</v>
       </c>
       <c r="D80">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L80" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"GLC", "ST", 11, "(4)"</v>
+        <v>"GLC", "ST", 8, "(3)"</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="N80" s="34">
         <v>137</v>
@@ -5084,11 +5179,31 @@
       <c r="S80" s="12"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D81"/>
+      <c r="A81" t="s">
+        <v>368</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D81">
+        <v>9</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>"GLC", "ST", 9, "(4)"</v>
+      </c>
       <c r="M81" s="20" t="s">
-        <v>516</v>
-      </c>
-      <c r="N81" s="34"/>
+        <v>509</v>
+      </c>
+      <c r="N81" s="34">
+        <v>137</v>
+      </c>
       <c r="O81" s="14"/>
       <c r="P81" s="14"/>
       <c r="Q81" s="12"/>
@@ -5097,32 +5212,29 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>210</v>
+        <v>368</v>
       </c>
       <c r="B82" t="s">
-        <v>202</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="L82" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-Bugla-Bry-1", "Sem(ST)+SBL", 1, "1", "(2)"</v>
+        <v>"GLC", "ST", 11, "(4)"</v>
       </c>
       <c r="M82" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="N82" s="33" t="s">
-        <v>337</v>
+        <v>510</v>
+      </c>
+      <c r="N82" s="34">
+        <v>137</v>
       </c>
       <c r="O82" s="14"/>
       <c r="P82" s="14"/>
@@ -5132,32 +5244,29 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>211</v>
+        <v>517</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>8</v>
+        <v>149</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D83">
+        <v>200</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="L83" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-Bugla-Bry-2", "SBL+Sem(PODG)", 1, "2", "(2)"</v>
+        <v>"GLC", "B-M", 200, "(N/A)"</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="N83" s="33" t="s">
-        <v>337</v>
+        <v>514</v>
+      </c>
+      <c r="N83" s="34">
+        <v>137</v>
       </c>
       <c r="O83" s="14"/>
       <c r="P83" s="14"/>
@@ -5167,16 +5276,17 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>312</v>
+        <v>518</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="D84"/>
       <c r="F84" s="2" t="s">
-        <v>312</v>
+        <v>518</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>7</v>
@@ -5186,13 +5296,13 @@
       </c>
       <c r="L84" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry", "PODG", 2, "1", "(1)"</v>
+        <v>"GLC-Szo", "Sem(odstep)", 1, "1", "(1)"</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="N84" s="33" t="s">
-        <v>337</v>
+        <v>521</v>
+      </c>
+      <c r="N84" s="34">
+        <v>137</v>
       </c>
       <c r="O84" s="14"/>
       <c r="P84" s="14"/>
@@ -5202,16 +5312,17 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>312</v>
+        <v>519</v>
       </c>
       <c r="B85" t="s">
-        <v>46</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="D85"/>
       <c r="F85" s="2" t="s">
-        <v>312</v>
+        <v>519</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>7</v>
@@ -5221,13 +5332,13 @@
       </c>
       <c r="L85" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry", "PODG", 1, "1", "(1)"</v>
+        <v>"Szo-GLC", "SBL(odstep)", 2, "1", "(1)"</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="N85" s="33" t="s">
-        <v>337</v>
+        <v>522</v>
+      </c>
+      <c r="N85" s="34">
+        <v>137</v>
       </c>
       <c r="O85" s="14"/>
       <c r="P85" s="14"/>
@@ -5237,29 +5348,29 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>303</v>
+        <v>210</v>
       </c>
       <c r="B86" t="s">
-        <v>304</v>
+        <v>202</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L86" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KO", "PODG+Sem(ST)", 2, "1", "(1)"</v>
+        <v>"KO-Bugla-Bry-1", "Sem(ST)+SBL", 1, "1", "(2)"</v>
       </c>
       <c r="M86" s="20" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="N86" s="33" t="s">
         <v>337</v>
@@ -5272,29 +5383,29 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="B87" t="s">
-        <v>305</v>
+        <v>107</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L87" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KO-Bry", "ST+Sem(PODG)", 3, "1", "(1)"</v>
+        <v>"KO-Bugla-Bry-2", "SBL+Sem(PODG)", 1, "2", "(2)"</v>
       </c>
       <c r="M87" s="20" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
       <c r="N87" s="33" t="s">
         <v>337</v>
@@ -5307,29 +5418,29 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>120</v>
+        <v>312</v>
       </c>
       <c r="B88" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>222</v>
+        <v>312</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L88" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KL-1", "SBL+POGP", 1, "1", "(2)"</v>
+        <v>"Bry", "PODG", 2, "1", "(1)"</v>
       </c>
       <c r="M88" s="20" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="N88" s="33" t="s">
         <v>337</v>
@@ -5342,29 +5453,29 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>121</v>
+        <v>312</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>223</v>
+        <v>312</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L89" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"Bry-KL-2", "SBL+Sem(ST)", 1, "2", "(2)"</v>
+        <v>"Bry", "PODG", 1, "1", "(1)"</v>
       </c>
       <c r="M89" s="20" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="N89" s="33" t="s">
         <v>337</v>
@@ -5377,13 +5488,13 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>303</v>
       </c>
       <c r="B90" t="s">
-        <v>67</v>
+        <v>304</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>224</v>
+        <v>110</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>8</v>
@@ -5392,14 +5503,14 @@
         <v>7</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L90" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-Bry-1", "SBL", 2, "1", "(2)"</v>
+        <v>"Bry-KO", "PODG+Sem(ST)", 2, "1", "(1)"</v>
       </c>
       <c r="M90" s="20" t="s">
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="N90" s="33" t="s">
         <v>337</v>
@@ -5412,29 +5523,29 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>313</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>225</v>
+        <v>109</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L91" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-Bry-2", "SBL+Sem(PODG)", 2, "2", "(2)"</v>
+        <v>"KO-Bry", "ST+Sem(PODG)", 3, "1", "(1)"</v>
       </c>
       <c r="M91" s="20" t="s">
-        <v>286</v>
+        <v>316</v>
       </c>
       <c r="N91" s="33" t="s">
         <v>337</v>
@@ -5447,26 +5558,29 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D92" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="H92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I92" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L92" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 1, "(2)"</v>
+        <v>"Bry-KL-1", "SBL+POGP", 1, "1", "(2)"</v>
       </c>
       <c r="M92" s="20" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="N92" s="33" t="s">
         <v>337</v>
@@ -5479,26 +5593,29 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D93" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="I93" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L93" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 2, "(2)"</v>
+        <v>"Bry-KL-2", "SBL+Sem(ST)", 1, "2", "(2)"</v>
       </c>
       <c r="M93" s="20" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="N93" s="33" t="s">
         <v>337</v>
@@ -5511,26 +5628,29 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L94" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL", "ST", 3, "(1)"</v>
+        <v>"KL-Bry-1", "SBL", 2, "1", "(2)"</v>
       </c>
       <c r="M94" s="20" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="N94" s="33" t="s">
         <v>337</v>
@@ -5543,32 +5663,32 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>370</v>
+        <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>416</v>
+        <v>107</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>373</v>
+        <v>225</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L95" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KL-MJ-1", "Sem(odstep)+PO(Piotrowice)", 1, "1", "(2)"</v>
+        <v>"KL-Bry-2", "SBL+Sem(PODG)", 2, "2", "(2)"</v>
       </c>
       <c r="M95" s="20" t="s">
-        <v>465</v>
+        <v>286</v>
       </c>
       <c r="N95" s="33" t="s">
-        <v>403</v>
+        <v>337</v>
       </c>
       <c r="O95" s="14"/>
       <c r="P95" s="14"/>
@@ -5578,32 +5698,29 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>372</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G96" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="E96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I96" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="L96" s="11" t="str">
-        <f t="shared" ref="L96:L122" si="2">IF(C96="",CONCATENATE($F$1,F96,$F$1,$G$1,$F$1,B96,$F$1,$G$1,G96,$G$1,$F$1,H96,$F$1,$G$1,$F$1,$B$1,I96,$C$1,$F$1),CONCATENATE($F$1,C96,$F$1,$G$1, $F$1,B96,$F$1,$G$1,D96,$G$1,$F$1,$B$1,E96,$C$1,$F$1))</f>
-        <v>"KL-MJ-2", "Sem(odstep)", 1, "2", "(2)"</v>
+        <f t="shared" si="1"/>
+        <v>"KL", "ST", 1, "(2)"</v>
       </c>
       <c r="M96" s="20" t="s">
-        <v>466</v>
+        <v>287</v>
       </c>
       <c r="N96" s="33" t="s">
-        <v>403</v>
+        <v>337</v>
       </c>
       <c r="O96" s="14"/>
       <c r="P96" s="14"/>
@@ -5613,29 +5730,29 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>399</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>400</v>
+        <v>112</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L97" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"MJ", "ST", 1, "(1)"</v>
+        <f t="shared" si="1"/>
+        <v>"KL", "ST", 2, "(2)"</v>
       </c>
       <c r="M97" s="20" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="N97" s="33" t="s">
-        <v>403</v>
+        <v>337</v>
       </c>
       <c r="O97" s="14"/>
       <c r="P97" s="14"/>
@@ -5645,29 +5762,29 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>399</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>400</v>
+        <v>112</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L98" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"MJ", "ST", 2, "(1)"</v>
+        <f t="shared" si="1"/>
+        <v>"KL", "ST", 3, "(1)"</v>
       </c>
       <c r="M98" s="20" t="s">
-        <v>468</v>
+        <v>289</v>
       </c>
       <c r="N98" s="33" t="s">
-        <v>403</v>
+        <v>337</v>
       </c>
       <c r="O98" s="14"/>
       <c r="P98" s="14"/>
@@ -5677,13 +5794,13 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="B99" t="s">
-        <v>372</v>
+        <v>416</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>7</v>
@@ -5692,14 +5809,14 @@
         <v>7</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L99" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"MJ-Mi", "Sem(odstep)", 1, "1", "(1)"</v>
+        <f t="shared" si="1"/>
+        <v>"KL-MJ-1", "Sem(odstep)+PO(Piotrowice)", 1, "1", "(2)"</v>
       </c>
       <c r="M99" s="20" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="N99" s="33" t="s">
         <v>403</v>
@@ -5712,26 +5829,29 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="D100" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>7</v>
+      <c r="H100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L100" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"Mi", "ST", 1, "(1)"</v>
+        <f t="shared" ref="L100:L126" si="2">IF(C100="",CONCATENATE($F$1,F100,$F$1,$G$1,$F$1,B100,$F$1,$G$1,G100,$G$1,$F$1,H100,$F$1,$G$1,$F$1,$B$1,I100,$C$1,$F$1),CONCATENATE($F$1,C100,$F$1,$G$1, $F$1,B100,$F$1,$G$1,D100,$G$1,$F$1,$B$1,E100,$C$1,$F$1))</f>
+        <v>"KL-MJ-2", "Sem(odstep)", 1, "2", "(2)"</v>
       </c>
       <c r="M100" s="20" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="N100" s="33" t="s">
         <v>403</v>
@@ -5744,26 +5864,26 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B101" t="s">
         <v>20</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>434</v>
+        <v>400</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L101" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mi", "ST", 2, "(1)"</v>
+        <v>"MJ", "ST", 1, "(1)"</v>
       </c>
       <c r="M101" s="20" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="N101" s="33" t="s">
         <v>403</v>
@@ -5776,32 +5896,29 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B102" t="s">
-        <v>417</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="G102" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="L102" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
+        <v>"MJ", "ST", 2, "(1)"</v>
       </c>
       <c r="M102" s="20" t="s">
-        <v>472</v>
+        <v>515</v>
       </c>
       <c r="N102" s="33" t="s">
-        <v>337</v>
+        <v>403</v>
       </c>
       <c r="O102" s="14"/>
       <c r="P102" s="14"/>
@@ -5811,32 +5928,32 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B103" t="s">
-        <v>67</v>
+        <v>372</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>419</v>
+        <v>7</v>
       </c>
       <c r="L103" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
+        <v>"MJ-Mi", "Sem(odstep)", 1, "1", "(1)"</v>
       </c>
       <c r="M103" s="20" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="N103" s="33" t="s">
-        <v>337</v>
+        <v>403</v>
       </c>
       <c r="O103" s="14"/>
       <c r="P103" s="14"/>
@@ -5846,32 +5963,29 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B104" t="s">
-        <v>67</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="G104" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H104" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>419</v>
+      <c r="E104" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L104" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
+        <v>"Mi", "ST", 1, "(2)"</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>474</v>
+        <v>516</v>
       </c>
       <c r="N104" s="33" t="s">
-        <v>337</v>
+        <v>403</v>
       </c>
       <c r="O104" s="14"/>
       <c r="P104" s="14"/>
@@ -5881,32 +5995,29 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B105" t="s">
-        <v>418</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="G105" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="L105" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
+        <v>"Mi", "ST", 2, "(1)"</v>
       </c>
       <c r="M105" s="20" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="N105" s="33" t="s">
-        <v>337</v>
+        <v>403</v>
       </c>
       <c r="O105" s="14"/>
       <c r="P105" s="14"/>
@@ -5916,29 +6027,29 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B106" t="s">
-        <v>67</v>
+        <v>417</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L106" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
+        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="N106" s="33" t="s">
         <v>337</v>
@@ -5951,29 +6062,29 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>419</v>
+        <v>8</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L107" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
+        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="N107" s="33" t="s">
         <v>337</v>
@@ -5986,29 +6097,29 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B108" t="s">
         <v>67</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>489</v>
+        <v>422</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L108" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
+        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="N108" s="33" t="s">
         <v>337</v>
@@ -6021,29 +6132,29 @@
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B109" t="s">
         <v>418</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>490</v>
+        <v>423</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L109" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
+        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="N109" s="33" t="s">
         <v>337</v>
@@ -6056,29 +6167,29 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B110" t="s">
         <v>67</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>491</v>
+        <v>424</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L110" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
+        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="N110" s="33" t="s">
         <v>337</v>
@@ -6091,29 +6202,29 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B111" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>492</v>
+        <v>425</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>9</v>
+        <v>419</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L111" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
+        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>497</v>
+        <v>475</v>
       </c>
       <c r="N111" s="33" t="s">
         <v>337</v>
@@ -6126,29 +6237,29 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B112" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L112" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
+        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="N112" s="33" t="s">
         <v>337</v>
@@ -6161,26 +6272,29 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="B113" t="s">
-        <v>46</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>105</v>
+        <v>418</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L113" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 1, "(N/A)"</v>
+        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>478</v>
+        <v>493</v>
       </c>
       <c r="N113" s="33" t="s">
         <v>337</v>
@@ -6193,26 +6307,32 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="B114" t="s">
-        <v>46</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D114" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="G114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>105</v>
+      <c r="H114" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L114" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 2, "(N/A)"</v>
+        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>479</v>
+        <v>494</v>
+      </c>
+      <c r="N114" s="33" t="s">
+        <v>337</v>
       </c>
       <c r="O114" s="14"/>
       <c r="P114" s="14"/>
@@ -6222,26 +6342,32 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B115" t="s">
-        <v>46</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>105</v>
+        <v>67</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L115" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 3, "(N/A)"</v>
+        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>480</v>
+        <v>495</v>
+      </c>
+      <c r="N115" s="33" t="s">
+        <v>337</v>
       </c>
       <c r="O115" s="14"/>
       <c r="P115" s="14"/>
@@ -6251,29 +6377,29 @@
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="B116" t="s">
-        <v>426</v>
+        <v>77</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>427</v>
+        <v>491</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="L116" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
+        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>481</v>
+        <v>496</v>
       </c>
       <c r="N116" s="33" t="s">
         <v>337</v>
@@ -6286,29 +6412,26 @@
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="B117" t="s">
-        <v>372</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H117" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I117" s="2" t="s">
-        <v>7</v>
+      <c r="E117" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="L117" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
+        <v>"Mc", "PODG", 1, "(N/A)"</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="N117" s="33" t="s">
         <v>337</v>
@@ -6321,29 +6444,26 @@
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>436</v>
+        <v>404</v>
       </c>
       <c r="B118" t="s">
-        <v>433</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="L118" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
+        <v>"Mc", "PODG", 2, "(N/A)"</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="N118" s="33" t="s">
         <v>337</v>
@@ -6356,26 +6476,26 @@
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
       <c r="B119" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>499</v>
+        <v>10</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L119" s="11" t="str">
-        <f t="shared" ref="L119:L121" si="3">IF(C119="",CONCATENATE($F$1,F119,$F$1,$G$1,$F$1,B119,$F$1,$G$1,G119,$G$1,$F$1,H119,$F$1,$G$1,$F$1,$B$1,I119,$C$1,$F$1),CONCATENATE($F$1,C119,$F$1,$G$1, $F$1,B119,$F$1,$G$1,D119,$G$1,$F$1,$B$1,E119,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 101, "(N/A)"</v>
+        <f t="shared" si="2"/>
+        <v>"Mc", "PODG", 3, "(N/A)"</v>
       </c>
       <c r="M119" s="20" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
       <c r="N119" s="33" t="s">
         <v>337</v>
@@ -6388,26 +6508,29 @@
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="B120" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>105</v>
+        <v>426</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L120" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>"Ty", "ST", 102, "(N/A)"</v>
+        <f t="shared" si="2"/>
+        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M120" s="20" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="N120" s="33" t="s">
         <v>337</v>
@@ -6420,26 +6543,29 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B121" t="s">
-        <v>20</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>105</v>
+        <v>372</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L121" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>"Ty", "ST", 108, "(N/A)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
       </c>
       <c r="M121" s="20" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="N121" s="33" t="s">
         <v>337</v>
@@ -6452,26 +6578,29 @@
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="B122" t="s">
-        <v>20</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D122" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H122" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E122" s="2" t="s">
-        <v>8</v>
+      <c r="I122" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L122" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty", "ST", 1, "(2)"</v>
+        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
       </c>
       <c r="M122" s="20" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="N122" s="33" t="s">
         <v>337</v>
@@ -6493,17 +6622,17 @@
         <v>428</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>8</v>
+        <v>497</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="L123" s="11" t="str">
-        <f t="shared" ref="L123:L126" si="4">IF(C123="",CONCATENATE($F$1,F123,$F$1,$G$1,$F$1,B123,$F$1,$G$1,G123,$G$1,$F$1,H123,$F$1,$G$1,$F$1,$B$1,I123,$C$1,$F$1),CONCATENATE($F$1,C123,$F$1,$G$1, $F$1,B123,$F$1,$G$1,D123,$G$1,$F$1,$B$1,E123,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 2, "(2)"</v>
+        <f t="shared" ref="L123:L125" si="3">IF(C123="",CONCATENATE($F$1,F123,$F$1,$G$1,$F$1,B123,$F$1,$G$1,G123,$G$1,$F$1,H123,$F$1,$G$1,$F$1,$B$1,I123,$C$1,$F$1),CONCATENATE($F$1,C123,$F$1,$G$1, $F$1,B123,$F$1,$G$1,D123,$G$1,$F$1,$B$1,E123,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 101, "(N/A)"</v>
       </c>
       <c r="M123" s="20" t="s">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="N123" s="33" t="s">
         <v>337</v>
@@ -6525,17 +6654,17 @@
         <v>428</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>430</v>
+        <v>498</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="L124" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>"Ty", "ST", 8, "(1)"</v>
+        <f t="shared" si="3"/>
+        <v>"Ty", "ST", 102, "(N/A)"</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>486</v>
+        <v>501</v>
       </c>
       <c r="N124" s="33" t="s">
         <v>337</v>
@@ -6557,17 +6686,17 @@
         <v>428</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>431</v>
+        <v>499</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="L125" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>"Ty", "ST", 7, "(3)"</v>
+        <f t="shared" si="3"/>
+        <v>"Ty", "ST", 108, "(N/A)"</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>487</v>
+        <v>502</v>
       </c>
       <c r="N125" s="33" t="s">
         <v>337</v>
@@ -6589,17 +6718,17 @@
         <v>428</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>432</v>
+        <v>7</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L126" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>"Ty", "ST", 9, "(3)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty", "ST", 1, "(2)"</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="N126" s="33" t="s">
         <v>337</v>
@@ -6612,32 +6741,29 @@
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>116</v>
+        <v>429</v>
       </c>
       <c r="B127" t="s">
-        <v>77</v>
-      </c>
-      <c r="F127" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I127" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L127" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
+        <f t="shared" ref="L127:L130" si="4">IF(C127="",CONCATENATE($F$1,F127,$F$1,$G$1,$F$1,B127,$F$1,$G$1,G127,$G$1,$F$1,H127,$F$1,$G$1,$F$1,$B$1,I127,$C$1,$F$1),CONCATENATE($F$1,C127,$F$1,$G$1, $F$1,B127,$F$1,$G$1,D127,$G$1,$F$1,$B$1,E127,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 2, "(2)"</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>290</v>
+        <v>483</v>
       </c>
       <c r="N127" s="33" t="s">
-        <v>7</v>
+        <v>337</v>
       </c>
       <c r="O127" s="14"/>
       <c r="P127" s="14"/>
@@ -6647,32 +6773,29 @@
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>117</v>
+        <v>429</v>
       </c>
       <c r="B128" t="s">
-        <v>77</v>
-      </c>
-      <c r="F128" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="G128" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H128" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E128" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I128" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="L128" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty", "ST", 8, "(1)"</v>
       </c>
       <c r="M128" s="20" t="s">
-        <v>291</v>
+        <v>484</v>
       </c>
       <c r="N128" s="33" t="s">
-        <v>7</v>
+        <v>337</v>
       </c>
       <c r="O128" s="14"/>
       <c r="P128" s="14"/>
@@ -6682,32 +6805,29 @@
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>118</v>
+        <v>429</v>
       </c>
       <c r="B129" t="s">
-        <v>77</v>
-      </c>
-      <c r="F129" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G129" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H129" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I129" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="L129" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty", "ST", 7, "(3)"</v>
       </c>
       <c r="M129" s="20" t="s">
-        <v>292</v>
+        <v>485</v>
       </c>
       <c r="N129" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O129" s="14"/>
       <c r="P129" s="14"/>
@@ -6717,32 +6837,29 @@
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>119</v>
+        <v>429</v>
       </c>
       <c r="B130" t="s">
-        <v>77</v>
-      </c>
-      <c r="F130" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H130" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I130" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L130" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty", "ST", 9, "(3)"</v>
       </c>
       <c r="M130" s="20" t="s">
-        <v>293</v>
+        <v>486</v>
       </c>
       <c r="N130" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O130" s="14"/>
       <c r="P130" s="14"/>
@@ -6752,26 +6869,29 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B131" t="s">
-        <v>20</v>
-      </c>
-      <c r="C131" t="s">
-        <v>144</v>
-      </c>
-      <c r="D131" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F131" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G131" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E131" s="2" t="s">
+      <c r="H131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I131" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L131" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 1, "(1)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M131" s="20" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="N131" s="33" t="s">
         <v>7</v>
@@ -6784,26 +6904,29 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B132" t="s">
-        <v>20</v>
-      </c>
-      <c r="C132" t="s">
-        <v>144</v>
-      </c>
-      <c r="D132" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F132" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G132" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E132" s="2" t="s">
+      <c r="H132" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I132" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L132" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 2, "(1)"</v>
+        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
       </c>
       <c r="M132" s="20" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="N132" s="33" t="s">
         <v>7</v>
@@ -6816,26 +6939,29 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B133" t="s">
-        <v>20</v>
-      </c>
-      <c r="C133" t="s">
-        <v>144</v>
-      </c>
-      <c r="D133" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F133" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E133" s="2" t="s">
-        <v>8</v>
+      <c r="H133" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L133" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 3, "(2)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
       </c>
       <c r="M133" s="20" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="N133" s="33" t="s">
         <v>338</v>
@@ -6848,26 +6974,29 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B134" t="s">
-        <v>20</v>
-      </c>
-      <c r="C134" t="s">
-        <v>144</v>
-      </c>
-      <c r="D134" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F134" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G134" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E134" s="2" t="s">
-        <v>8</v>
+      <c r="H134" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I134" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L134" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 4, "(2)"</v>
+        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
       </c>
       <c r="M134" s="20" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="N134" s="33" t="s">
         <v>338</v>
@@ -6879,12 +7008,30 @@
       <c r="S134" s="12"/>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>143</v>
+      </c>
+      <c r="B135" t="s">
+        <v>20</v>
+      </c>
+      <c r="C135" t="s">
+        <v>144</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="L135" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"", "", , "", "()"</v>
+        <v>"KZ", "ST", 1, "(1)"</v>
       </c>
       <c r="M135" s="20" t="s">
-        <v>184</v>
+        <v>294</v>
+      </c>
+      <c r="N135" s="33" t="s">
+        <v>7</v>
       </c>
       <c r="O135" s="14"/>
       <c r="P135" s="14"/>
@@ -6893,12 +7040,30 @@
       <c r="S135" s="12"/>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>143</v>
+      </c>
+      <c r="B136" t="s">
+        <v>20</v>
+      </c>
+      <c r="C136" t="s">
+        <v>144</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="L136" s="11" t="str">
-        <f t="shared" ref="L136:L199" si="5">IF(C136="",CONCATENATE($F$1,F136,$F$1,$G$1,$F$1,B136,$F$1,$G$1,G136,$G$1,$F$1,H136,$F$1,$G$1,$F$1,$B$1,I136,$C$1,$F$1),CONCATENATE($F$1,C136,$F$1,$G$1, $F$1,B136,$F$1,$G$1,D136,$G$1,$F$1,$B$1,E136,$C$1,$F$1))</f>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 2, "(1)"</v>
       </c>
       <c r="M136" s="20" t="s">
-        <v>184</v>
+        <v>295</v>
+      </c>
+      <c r="N136" s="33" t="s">
+        <v>7</v>
       </c>
       <c r="O136" s="14"/>
       <c r="P136" s="14"/>
@@ -6907,12 +7072,30 @@
       <c r="S136" s="12"/>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>143</v>
+      </c>
+      <c r="B137" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" t="s">
+        <v>144</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L137" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 3, "(2)"</v>
       </c>
       <c r="M137" s="20" t="s">
-        <v>184</v>
+        <v>296</v>
+      </c>
+      <c r="N137" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O137" s="14"/>
       <c r="P137" s="14"/>
@@ -6921,12 +7104,30 @@
       <c r="S137" s="12"/>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>143</v>
+      </c>
+      <c r="B138" t="s">
+        <v>20</v>
+      </c>
+      <c r="C138" t="s">
+        <v>144</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L138" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 4, "(2)"</v>
       </c>
       <c r="M138" s="20" t="s">
-        <v>184</v>
+        <v>297</v>
+      </c>
+      <c r="N138" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O138" s="14"/>
       <c r="P138" s="14"/>
@@ -6935,12 +7136,27 @@
       <c r="S138" s="12"/>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>527</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I139" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L139" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ-SG", "", 1, "1", "(3)"</v>
       </c>
       <c r="M139" s="20" t="s">
-        <v>184</v>
+        <v>529</v>
       </c>
       <c r="O139" s="14"/>
       <c r="P139" s="14"/>
@@ -6949,12 +7165,27 @@
       <c r="S139" s="12"/>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>528</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I140" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L140" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" ref="L140:L203" si="5">IF(C140="",CONCATENATE($F$1,F140,$F$1,$G$1,$F$1,B140,$F$1,$G$1,G140,$G$1,$F$1,H140,$F$1,$G$1,$F$1,$B$1,I140,$C$1,$F$1),CONCATENATE($F$1,C140,$F$1,$G$1, $F$1,B140,$F$1,$G$1,D140,$G$1,$F$1,$B$1,E140,$C$1,$F$1))</f>
+        <v>"SG-KZ", "", 2, "3", "(3)"</v>
       </c>
       <c r="M140" s="20" t="s">
-        <v>184</v>
+        <v>530</v>
       </c>
       <c r="O140" s="14"/>
       <c r="P140" s="14"/>
@@ -6963,12 +7194,30 @@
       <c r="S140" s="12"/>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>523</v>
+      </c>
+      <c r="B141" t="s">
+        <v>67</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L141" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <v>"KZ-Szb_1", "SBL", 3, "2", "(2)"</v>
       </c>
       <c r="M141" s="20" t="s">
-        <v>184</v>
+        <v>531</v>
       </c>
       <c r="O141" s="14"/>
       <c r="P141" s="14"/>
@@ -6977,12 +7226,30 @@
       <c r="S141" s="12"/>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>524</v>
+      </c>
+      <c r="B142" t="s">
+        <v>77</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L142" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <v>"Szb-KZ_3", "SBL+Sem(ST)", 4, "1", "(3)"</v>
       </c>
       <c r="M142" s="20" t="s">
-        <v>184</v>
+        <v>532</v>
       </c>
       <c r="O142" s="14"/>
       <c r="P142" s="14"/>
@@ -7082,6 +7349,11 @@
       <c r="M149" s="20" t="s">
         <v>184</v>
       </c>
+      <c r="O149" s="14"/>
+      <c r="P149" s="14"/>
+      <c r="Q149" s="12"/>
+      <c r="R149" s="12"/>
+      <c r="S149" s="12"/>
     </row>
     <row r="150" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L150" s="11" t="str">
@@ -7091,6 +7363,11 @@
       <c r="M150" s="20" t="s">
         <v>184</v>
       </c>
+      <c r="O150" s="14"/>
+      <c r="P150" s="14"/>
+      <c r="Q150" s="12"/>
+      <c r="R150" s="12"/>
+      <c r="S150" s="12"/>
     </row>
     <row r="151" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L151" s="11" t="str">
@@ -7100,6 +7377,11 @@
       <c r="M151" s="20" t="s">
         <v>184</v>
       </c>
+      <c r="O151" s="14"/>
+      <c r="P151" s="14"/>
+      <c r="Q151" s="12"/>
+      <c r="R151" s="12"/>
+      <c r="S151" s="12"/>
     </row>
     <row r="152" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L152" s="11" t="str">
@@ -7109,6 +7391,11 @@
       <c r="M152" s="20" t="s">
         <v>184</v>
       </c>
+      <c r="O152" s="14"/>
+      <c r="P152" s="14"/>
+      <c r="Q152" s="12"/>
+      <c r="R152" s="12"/>
+      <c r="S152" s="12"/>
     </row>
     <row r="153" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L153" s="11" t="str">
@@ -7535,7 +7822,7 @@
     </row>
     <row r="200" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L200" s="11" t="str">
-        <f t="shared" ref="L200:L263" si="6">IF(C200="",CONCATENATE($F$1,F200,$F$1,$G$1,$F$1,B200,$F$1,$G$1,G200,$G$1,$F$1,H200,$F$1,$G$1,$F$1,$B$1,I200,$C$1,$F$1),CONCATENATE($F$1,C200,$F$1,$G$1, $F$1,B200,$F$1,$G$1,D200,$G$1,$F$1,$B$1,E200,$C$1,$F$1))</f>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M200" s="20" t="s">
@@ -7544,7 +7831,7 @@
     </row>
     <row r="201" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L201" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M201" s="20" t="s">
@@ -7553,7 +7840,7 @@
     </row>
     <row r="202" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L202" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M202" s="20" t="s">
@@ -7562,7 +7849,7 @@
     </row>
     <row r="203" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L203" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M203" s="20" t="s">
@@ -7571,7 +7858,7 @@
     </row>
     <row r="204" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L204" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="L204:L267" si="6">IF(C204="",CONCATENATE($F$1,F204,$F$1,$G$1,$F$1,B204,$F$1,$G$1,G204,$G$1,$F$1,H204,$F$1,$G$1,$F$1,$B$1,I204,$C$1,$F$1),CONCATENATE($F$1,C204,$F$1,$G$1, $F$1,B204,$F$1,$G$1,D204,$G$1,$F$1,$B$1,E204,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M204" s="20" t="s">
@@ -8111,7 +8398,7 @@
     </row>
     <row r="264" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L264" s="11" t="str">
-        <f t="shared" ref="L264:L327" si="7">IF(C264="",CONCATENATE($F$1,F264,$F$1,$G$1,$F$1,B264,$F$1,$G$1,G264,$G$1,$F$1,H264,$F$1,$G$1,$F$1,$B$1,I264,$C$1,$F$1),CONCATENATE($F$1,C264,$F$1,$G$1, $F$1,B264,$F$1,$G$1,D264,$G$1,$F$1,$B$1,E264,$C$1,$F$1))</f>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M264" s="20" t="s">
@@ -8120,7 +8407,7 @@
     </row>
     <row r="265" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L265" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M265" s="20" t="s">
@@ -8129,7 +8416,7 @@
     </row>
     <row r="266" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L266" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M266" s="20" t="s">
@@ -8138,7 +8425,7 @@
     </row>
     <row r="267" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L267" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M267" s="20" t="s">
@@ -8147,7 +8434,7 @@
     </row>
     <row r="268" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L268" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L268:L331" si="7">IF(C268="",CONCATENATE($F$1,F268,$F$1,$G$1,$F$1,B268,$F$1,$G$1,G268,$G$1,$F$1,H268,$F$1,$G$1,$F$1,$B$1,I268,$C$1,$F$1),CONCATENATE($F$1,C268,$F$1,$G$1, $F$1,B268,$F$1,$G$1,D268,$G$1,$F$1,$B$1,E268,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M268" s="20" t="s">
@@ -8687,7 +8974,7 @@
     </row>
     <row r="328" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L328" s="11" t="str">
-        <f t="shared" ref="L328:L391" si="8">IF(C328="",CONCATENATE($F$1,F328,$F$1,$G$1,$F$1,B328,$F$1,$G$1,G328,$G$1,$F$1,H328,$F$1,$G$1,$F$1,$B$1,I328,$C$1,$F$1),CONCATENATE($F$1,C328,$F$1,$G$1, $F$1,B328,$F$1,$G$1,D328,$G$1,$F$1,$B$1,E328,$C$1,$F$1))</f>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M328" s="20" t="s">
@@ -8696,7 +8983,7 @@
     </row>
     <row r="329" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L329" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M329" s="20" t="s">
@@ -8705,7 +8992,7 @@
     </row>
     <row r="330" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L330" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M330" s="20" t="s">
@@ -8714,7 +9001,7 @@
     </row>
     <row r="331" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L331" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M331" s="20" t="s">
@@ -8723,7 +9010,7 @@
     </row>
     <row r="332" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L332" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L332:L395" si="8">IF(C332="",CONCATENATE($F$1,F332,$F$1,$G$1,$F$1,B332,$F$1,$G$1,G332,$G$1,$F$1,H332,$F$1,$G$1,$F$1,$B$1,I332,$C$1,$F$1),CONCATENATE($F$1,C332,$F$1,$G$1, $F$1,B332,$F$1,$G$1,D332,$G$1,$F$1,$B$1,E332,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M332" s="20" t="s">
@@ -9263,7 +9550,7 @@
     </row>
     <row r="392" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L392" s="11" t="str">
-        <f t="shared" ref="L392:L400" si="9">IF(C392="",CONCATENATE($F$1,F392,$F$1,$G$1,$F$1,B392,$F$1,$G$1,G392,$G$1,$F$1,H392,$F$1,$G$1,$F$1,$B$1,I392,$C$1,$F$1),CONCATENATE($F$1,C392,$F$1,$G$1, $F$1,B392,$F$1,$G$1,D392,$G$1,$F$1,$B$1,E392,$C$1,$F$1))</f>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M392" s="20" t="s">
@@ -9272,7 +9559,7 @@
     </row>
     <row r="393" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L393" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M393" s="20" t="s">
@@ -9281,7 +9568,7 @@
     </row>
     <row r="394" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L394" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M394" s="20" t="s">
@@ -9290,7 +9577,7 @@
     </row>
     <row r="395" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L395" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M395" s="20" t="s">
@@ -9299,7 +9586,7 @@
     </row>
     <row r="396" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L396" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="L396:L404" si="9">IF(C396="",CONCATENATE($F$1,F396,$F$1,$G$1,$F$1,B396,$F$1,$G$1,G396,$G$1,$F$1,H396,$F$1,$G$1,$F$1,$B$1,I396,$C$1,$F$1),CONCATENATE($F$1,C396,$F$1,$G$1, $F$1,B396,$F$1,$G$1,D396,$G$1,$F$1,$B$1,E396,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M396" s="20" t="s">
@@ -9339,6 +9626,42 @@
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M400" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="401" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L401" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M401" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="402" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L402" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M402" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="403" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L403" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M403" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="404" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L404" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M404" s="20" t="s">
         <v>184</v>
       </c>
     </row>
@@ -13139,12 +13462,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CD5458B81A8B2B4B92FF87D810305C72" ma:contentTypeVersion="10" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="94af6a530ab954c472b36ae778f182c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bcc645c8-4b47-4a2e-89eb-d5bbcced8466" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ef69444b0b6df3a2aca9b298e9665c5" ns3:_="">
     <xsd:import namespace="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
@@ -13328,6 +13645,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2395D0C0-9628-4C07-92CD-D40200588B84}">
   <ds:schemaRefs>
@@ -13337,22 +13660,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80CA5C0B-23D0-4CD7-AF29-D46F01A941B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BBCE1FC-4F3C-4CE6-A38A-EF0D12121C1C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13368,4 +13675,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80CA5C0B-23D0-4CD7-AF29-D46F01A941B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
full network paths and blocks
</commit_message>
<xml_diff>
--- a/data/Spis odcinków_KO-CB-KZ-KL.xlsx
+++ b/data/Spis odcinków_KO-CB-KZ-KL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\railways_dispatching_silesia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADCE2CA-8EEA-457B-9A50-D8AD2AB9B8A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF151E6-60FE-45D9-B42E-AD889AE151D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="555">
   <si>
     <t>Katowice</t>
   </si>
@@ -1563,21 +1563,6 @@
     <t>"GLC", "ST", 11, "(4)"</t>
   </si>
   <si>
-    <t>"CM-CB", "SBL+Sem(ST)", 2, "1", "(1)"</t>
-  </si>
-  <si>
-    <t>"RCB-ZZ-2", "SBL+PO(Ruda Śląska)", 1, "2", "(4)"</t>
-  </si>
-  <si>
-    <t>"ZZ-RCB-3", "SBL+PO(Ruda Śląska)", 2, "3", "(4)"</t>
-  </si>
-  <si>
-    <t>"GLC(KS)", "B-M", 200, "(N/A)"</t>
-  </si>
-  <si>
-    <t>"MJ", "ST", 3, "(2)"</t>
-  </si>
-  <si>
     <t>"Mi", "ST", 1, "(2)"</t>
   </si>
   <si>
@@ -1605,30 +1590,12 @@
     <t>Szb-KZ</t>
   </si>
   <si>
-    <t>KZ-Szb_1</t>
-  </si>
-  <si>
-    <t>Szb-KZ_3</t>
-  </si>
-  <si>
     <t>KZ-SG</t>
   </si>
   <si>
     <t>SG-KZ</t>
   </si>
   <si>
-    <t>"KZ-SG", "", 1, "1", "(3)"</t>
-  </si>
-  <si>
-    <t>"SG-KZ", "", 2, "3", "(3)"</t>
-  </si>
-  <si>
-    <t>"KZ-Szb_1", "SBL", 3, "2", "(2)"</t>
-  </si>
-  <si>
-    <t>"Szb-KZ_3", "SBL+Sem(ST)", 4, "1", "(3)"</t>
-  </si>
-  <si>
     <t>CM-CS</t>
   </si>
   <si>
@@ -1642,6 +1609,90 @@
   </si>
   <si>
     <t>"CS-CM", "Sem(odstęp)", 2, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"SG-KZ", "SBL", 1, "1", "(3)"</t>
+  </si>
+  <si>
+    <t>"KZ-SG", "SBL+Sem(ST)", 2, "3", "(3)"</t>
+  </si>
+  <si>
+    <t>Szb-KZ-3</t>
+  </si>
+  <si>
+    <t>"Szb-KZ-3", "SBL", 3, "2", "(2)"</t>
+  </si>
+  <si>
+    <t>KZ-Szb-1</t>
+  </si>
+  <si>
+    <t>"KZ-Szb-1", "SBL+Sem(ST)", 4, "1", "(3)"</t>
+  </si>
+  <si>
+    <t>Mi-ŁGB</t>
+  </si>
+  <si>
+    <t>Mi_ŁGB</t>
+  </si>
+  <si>
+    <t>"Mi_ŁGB", "Sem(odstęp)", 1, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"CM-CB", "SBL+Sem(ST)", 1, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</t>
+  </si>
+  <si>
+    <t>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</t>
+  </si>
+  <si>
+    <t>"GLC", "B-M", 200, "(N/A)"</t>
+  </si>
+  <si>
+    <t>"MJ", "ST", 2, "(1)"</t>
+  </si>
+  <si>
+    <t>Ty-Kob</t>
+  </si>
+  <si>
+    <t>Kob-Ty</t>
+  </si>
+  <si>
+    <t>Ty-Kob-1</t>
+  </si>
+  <si>
+    <t>Kob-Ty-6</t>
+  </si>
+  <si>
+    <t>Ty-ŁŚ</t>
+  </si>
+  <si>
+    <t>Ty-Tmo</t>
+  </si>
+  <si>
+    <t>Tmo</t>
+  </si>
+  <si>
+    <t>TMo-Ty</t>
+  </si>
+  <si>
+    <t>"Ty-Kob-1", "SBL", 1, "1", "(6)"</t>
+  </si>
+  <si>
+    <t>"Kob-Ty-6", "SBL+Sem(ST)", 2, "6", "(6)"</t>
+  </si>
+  <si>
+    <t>"Ty-ŁŚ", "Sem(odstep)", 1, "1", "(1)"</t>
+  </si>
+  <si>
+    <t>"TMo-Ty", "Sem(odstęp)", 2, "1", "(1)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ty-TMo </t>
+  </si>
+  <si>
+    <t>"Ty-TMo ", "SBL", 1, "1", "(2)"</t>
   </si>
 </sst>
 </file>
@@ -1830,7 +1881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1904,6 +1955,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -2219,10 +2271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM404"/>
+  <dimension ref="A1:AM410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M84" sqref="M84:M85"/>
+    <sheetView tabSelected="1" topLeftCell="M118" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M132" sqref="M132:M136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3161,7 @@
       </c>
       <c r="F23" s="17"/>
       <c r="L23" s="11" t="str">
-        <f t="shared" ref="L23:L139" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
+        <f t="shared" ref="L23:L145" si="1">IF(C23="",CONCATENATE($F$1,F23,$F$1,$G$1,$F$1,B23,$F$1,$G$1,G23,$G$1,$F$1,H23,$F$1,$G$1,$F$1,$B$1,I23,$C$1,$F$1),CONCATENATE($F$1,C23,$F$1,$G$1, $F$1,B23,$F$1,$G$1,D23,$G$1,$F$1,$B$1,E23,$C$1,$F$1))</f>
         <v>"KO", "ST-M", 1114, "(N/A)"</v>
       </c>
       <c r="M23" s="11" t="s">
@@ -3853,7 +3905,7 @@
         <v>"CM-CB", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>511</v>
+        <v>536</v>
       </c>
       <c r="N42" s="33" t="s">
         <v>336</v>
@@ -3930,14 +3982,14 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="B45" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="D45"/>
       <c r="F45" s="2" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>7</v>
@@ -3953,7 +4005,7 @@
         <v>"CM-CS", "Sem(odstęp)", 1, "1", "(1)"</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
@@ -3963,14 +4015,14 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="B46" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="D46"/>
       <c r="F46" s="2" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>8</v>
@@ -3986,7 +4038,7 @@
         <v>"CS-CM", "Sem(odstęp)", 2, "1", "(1)"</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
@@ -4335,7 +4387,7 @@
         <v>"RCB-ZZ-2", "SBL+PO(Świętochłowice)", 1, "2", "(4)"</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
       <c r="N56" s="34">
         <v>137</v>
@@ -4515,7 +4567,7 @@
         <v>"ZZ-RCB-3", "SBL+PO(Świętochłowice)", 2, "3", "(4)"</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>513</v>
+        <v>538</v>
       </c>
       <c r="N61" s="34">
         <v>137</v>
@@ -5244,7 +5296,7 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="B83" t="s">
         <v>149</v>
@@ -5263,7 +5315,7 @@
         <v>"GLC", "B-M", 200, "(N/A)"</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>514</v>
+        <v>539</v>
       </c>
       <c r="N83" s="34">
         <v>137</v>
@@ -5276,14 +5328,14 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B84" t="s">
         <v>372</v>
       </c>
       <c r="D84"/>
       <c r="F84" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>7</v>
@@ -5299,7 +5351,7 @@
         <v>"GLC-Szo", "Sem(odstep)", 1, "1", "(1)"</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="N84" s="34">
         <v>137</v>
@@ -5312,14 +5364,14 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B85" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="D85"/>
       <c r="F85" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>8</v>
@@ -5335,7 +5387,7 @@
         <v>"Szo-GLC", "SBL(odstep)", 2, "1", "(1)"</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="N85" s="34">
         <v>137</v>
@@ -5847,7 +5899,7 @@
         <v>8</v>
       </c>
       <c r="L100" s="11" t="str">
-        <f t="shared" ref="L100:L126" si="2">IF(C100="",CONCATENATE($F$1,F100,$F$1,$G$1,$F$1,B100,$F$1,$G$1,G100,$G$1,$F$1,H100,$F$1,$G$1,$F$1,$B$1,I100,$C$1,$F$1),CONCATENATE($F$1,C100,$F$1,$G$1, $F$1,B100,$F$1,$G$1,D100,$G$1,$F$1,$B$1,E100,$C$1,$F$1))</f>
+        <f t="shared" ref="L100:L127" si="2">IF(C100="",CONCATENATE($F$1,F100,$F$1,$G$1,$F$1,B100,$F$1,$G$1,G100,$G$1,$F$1,H100,$F$1,$G$1,$F$1,$B$1,I100,$C$1,$F$1),CONCATENATE($F$1,C100,$F$1,$G$1, $F$1,B100,$F$1,$G$1,D100,$G$1,$F$1,$B$1,E100,$C$1,$F$1))</f>
         <v>"KL-MJ-2", "Sem(odstep)", 1, "2", "(2)"</v>
       </c>
       <c r="M100" s="20" t="s">
@@ -5915,7 +5967,7 @@
         <v>"MJ", "ST", 2, "(1)"</v>
       </c>
       <c r="M102" s="20" t="s">
-        <v>515</v>
+        <v>540</v>
       </c>
       <c r="N102" s="33" t="s">
         <v>403</v>
@@ -5982,7 +6034,7 @@
         <v>"Mi", "ST", 1, "(2)"</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="N104" s="33" t="s">
         <v>403</v>
@@ -6027,13 +6079,13 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>405</v>
+        <v>533</v>
       </c>
       <c r="B106" t="s">
-        <v>417</v>
+        <v>524</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>420</v>
+        <v>534</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>7</v>
@@ -6042,17 +6094,14 @@
         <v>7</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>419</v>
+        <v>7</v>
       </c>
       <c r="L106" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
+        <v>"Mi_ŁGB", "Sem(odstęp)", 1, "1", "(1)"</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>470</v>
-      </c>
-      <c r="N106" s="33" t="s">
-        <v>337</v>
+        <v>535</v>
       </c>
       <c r="O106" s="14"/>
       <c r="P106" s="14"/>
@@ -6062,29 +6111,29 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>417</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L107" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
+        <v>"KL-Mc-1", "SBL+PO(Piotrowice)", 1, "1", "(6)"</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N107" s="33" t="s">
         <v>337</v>
@@ -6097,29 +6146,29 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B108" t="s">
         <v>67</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L108" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
+        <v>"KL-Mc-2", "SBL", 1, "2", "(6)"</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N108" s="33" t="s">
         <v>337</v>
@@ -6132,29 +6181,29 @@
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B109" t="s">
-        <v>418</v>
+        <v>67</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L109" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
+        <v>"KL-Mc-3", "SBL", 1, "3", "(6)"</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="N109" s="33" t="s">
         <v>337</v>
@@ -6167,29 +6216,29 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B110" t="s">
-        <v>67</v>
+        <v>418</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L110" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
+        <v>"KL-Mc-4", "SBL+PO(Podlesie)", 1, "4", "(6)"</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N110" s="33" t="s">
         <v>337</v>
@@ -6202,29 +6251,29 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B111" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>419</v>
+        <v>113</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>419</v>
       </c>
       <c r="L111" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
+        <v>"KL-Mc-5", "SBL", 1, "5", "(6)"</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="N111" s="33" t="s">
         <v>337</v>
@@ -6237,29 +6286,29 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B112" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>113</v>
+        <v>419</v>
       </c>
       <c r="L112" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
+        <v>"KL-Mc-6", "SBL+Sem(PODG)", 1, "6", "(6)"</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="N112" s="33" t="s">
         <v>337</v>
@@ -6272,29 +6321,29 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B113" t="s">
-        <v>418</v>
+        <v>67</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L113" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
+        <v>"Mc-KL-1", "SBL", 2, "1", "(5)"</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N113" s="33" t="s">
         <v>337</v>
@@ -6307,29 +6356,29 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B114" t="s">
-        <v>67</v>
+        <v>418</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L114" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
+        <v>"Mc-KL-2", "SBL+PO(Podlesie)", 2, "2", "(5)"</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N114" s="33" t="s">
         <v>337</v>
@@ -6342,29 +6391,29 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B115" t="s">
         <v>67</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L115" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
+        <v>"Mc-KL-3", "SBL", 2, "3", "(5)"</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N115" s="33" t="s">
         <v>337</v>
@@ -6377,29 +6426,29 @@
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B116" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>113</v>
       </c>
       <c r="L116" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
+        <v>"Mc-KL-4", "SBL", 2, "4", "(5)"</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N116" s="33" t="s">
         <v>337</v>
@@ -6412,26 +6461,29 @@
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="B117" t="s">
-        <v>46</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>105</v>
+        <v>77</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="L117" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 1, "(N/A)"</v>
+        <v>"Mc-KL-5", "SBL+Sem(ST)", 2, "5", "(5)"</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>476</v>
+        <v>496</v>
       </c>
       <c r="N117" s="33" t="s">
         <v>337</v>
@@ -6453,17 +6505,17 @@
         <v>404</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L118" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 2, "(N/A)"</v>
+        <v>"Mc", "PODG", 1, "(N/A)"</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N118" s="33" t="s">
         <v>337</v>
@@ -6485,17 +6537,17 @@
         <v>404</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L119" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc", "PODG", 3, "(N/A)"</v>
+        <v>"Mc", "PODG", 2, "(N/A)"</v>
       </c>
       <c r="M119" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N119" s="33" t="s">
         <v>337</v>
@@ -6508,29 +6560,26 @@
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>438</v>
+        <v>404</v>
       </c>
       <c r="B120" t="s">
-        <v>426</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I120" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="L120" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
+        <v>"Mc", "PODG", 3, "(N/A)"</v>
       </c>
       <c r="M120" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N120" s="33" t="s">
         <v>337</v>
@@ -6543,16 +6592,16 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B121" t="s">
-        <v>372</v>
+        <v>426</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>7</v>
@@ -6562,10 +6611,10 @@
       </c>
       <c r="L121" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
+        <v>"Mc-Ty", "Sem(odstep)+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M121" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N121" s="33" t="s">
         <v>337</v>
@@ -6578,16 +6627,16 @@
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B122" t="s">
-        <v>433</v>
+        <v>372</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>435</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>7</v>
@@ -6597,10 +6646,10 @@
       </c>
       <c r="L122" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
+        <v>"Ty-Mc", "Sem(odstep)", 2, "1", "(1)"</v>
       </c>
       <c r="M122" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N122" s="33" t="s">
         <v>337</v>
@@ -6613,26 +6662,29 @@
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="B123" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>105</v>
+        <v>433</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L123" s="11" t="str">
-        <f t="shared" ref="L123:L125" si="3">IF(C123="",CONCATENATE($F$1,F123,$F$1,$G$1,$F$1,B123,$F$1,$G$1,G123,$G$1,$F$1,H123,$F$1,$G$1,$F$1,$B$1,I123,$C$1,$F$1),CONCATENATE($F$1,C123,$F$1,$G$1, $F$1,B123,$F$1,$G$1,D123,$G$1,$F$1,$B$1,E123,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 101, "(N/A)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty-Mc", "Sem(odstep)+Sem(PODG)", 3, "1", "(1)"</v>
       </c>
       <c r="M123" s="20" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="N123" s="33" t="s">
         <v>337</v>
@@ -6654,17 +6706,17 @@
         <v>428</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L124" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>"Ty", "ST", 102, "(N/A)"</v>
+        <f t="shared" ref="L124:L126" si="3">IF(C124="",CONCATENATE($F$1,F124,$F$1,$G$1,$F$1,B124,$F$1,$G$1,G124,$G$1,$F$1,H124,$F$1,$G$1,$F$1,$B$1,I124,$C$1,$F$1),CONCATENATE($F$1,C124,$F$1,$G$1, $F$1,B124,$F$1,$G$1,D124,$G$1,$F$1,$B$1,E124,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 101, "(N/A)"</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="N124" s="33" t="s">
         <v>337</v>
@@ -6686,17 +6738,17 @@
         <v>428</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>105</v>
       </c>
       <c r="L125" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>"Ty", "ST", 108, "(N/A)"</v>
+        <v>"Ty", "ST", 102, "(N/A)"</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N125" s="33" t="s">
         <v>337</v>
@@ -6718,17 +6770,17 @@
         <v>428</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>7</v>
+        <v>499</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="L126" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>"Ty", "ST", 1, "(2)"</v>
+        <f t="shared" si="3"/>
+        <v>"Ty", "ST", 108, "(N/A)"</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>482</v>
+        <v>502</v>
       </c>
       <c r="N126" s="33" t="s">
         <v>337</v>
@@ -6750,17 +6802,17 @@
         <v>428</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L127" s="11" t="str">
-        <f t="shared" ref="L127:L130" si="4">IF(C127="",CONCATENATE($F$1,F127,$F$1,$G$1,$F$1,B127,$F$1,$G$1,G127,$G$1,$F$1,H127,$F$1,$G$1,$F$1,$B$1,I127,$C$1,$F$1),CONCATENATE($F$1,C127,$F$1,$G$1, $F$1,B127,$F$1,$G$1,D127,$G$1,$F$1,$B$1,E127,$C$1,$F$1))</f>
-        <v>"Ty", "ST", 2, "(2)"</v>
+        <f t="shared" si="2"/>
+        <v>"Ty", "ST", 1, "(2)"</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N127" s="33" t="s">
         <v>337</v>
@@ -6782,17 +6834,17 @@
         <v>428</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>430</v>
+        <v>8</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L128" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>"Ty", "ST", 8, "(1)"</v>
+        <f t="shared" ref="L128:L136" si="4">IF(C128="",CONCATENATE($F$1,F128,$F$1,$G$1,$F$1,B128,$F$1,$G$1,G128,$G$1,$F$1,H128,$F$1,$G$1,$F$1,$B$1,I128,$C$1,$F$1),CONCATENATE($F$1,C128,$F$1,$G$1, $F$1,B128,$F$1,$G$1,D128,$G$1,$F$1,$B$1,E128,$C$1,$F$1))</f>
+        <v>"Ty", "ST", 2, "(2)"</v>
       </c>
       <c r="M128" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N128" s="33" t="s">
         <v>337</v>
@@ -6814,17 +6866,17 @@
         <v>428</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L129" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>"Ty", "ST", 7, "(3)"</v>
+        <v>"Ty", "ST", 8, "(1)"</v>
       </c>
       <c r="M129" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N129" s="33" t="s">
         <v>337</v>
@@ -6846,17 +6898,17 @@
         <v>428</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L130" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>"Ty", "ST", 9, "(3)"</v>
+        <v>"Ty", "ST", 7, "(3)"</v>
       </c>
       <c r="M130" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N130" s="33" t="s">
         <v>337</v>
@@ -6869,32 +6921,29 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>116</v>
+        <v>429</v>
       </c>
       <c r="B131" t="s">
-        <v>77</v>
-      </c>
-      <c r="F131" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G131" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I131" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L131" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty", "ST", 9, "(3)"</v>
       </c>
       <c r="M131" s="20" t="s">
-        <v>290</v>
+        <v>486</v>
       </c>
       <c r="N131" s="33" t="s">
-        <v>7</v>
+        <v>337</v>
       </c>
       <c r="O131" s="14"/>
       <c r="P131" s="14"/>
@@ -6904,32 +6953,29 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>117</v>
+        <v>541</v>
       </c>
       <c r="B132" t="s">
-        <v>77</v>
-      </c>
-      <c r="F132" s="31" t="s">
-        <v>115</v>
+        <v>67</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>543</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="L132" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty-Kob-1", "SBL", 1, "1", "(6)"</v>
       </c>
       <c r="M132" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N132" s="33" t="s">
-        <v>7</v>
+        <v>549</v>
       </c>
       <c r="O132" s="14"/>
       <c r="P132" s="14"/>
@@ -6939,32 +6985,29 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>118</v>
+        <v>542</v>
       </c>
       <c r="B133" t="s">
         <v>77</v>
       </c>
-      <c r="F133" s="31" t="s">
-        <v>114</v>
+      <c r="F133" s="2" t="s">
+        <v>544</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="L133" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Kob-Ty-6", "SBL+Sem(ST)", 2, "6", "(6)"</v>
       </c>
       <c r="M133" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="N133" s="33" t="s">
-        <v>338</v>
+        <v>550</v>
       </c>
       <c r="O133" s="14"/>
       <c r="P133" s="14"/>
@@ -6974,16 +7017,16 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>119</v>
+        <v>545</v>
       </c>
       <c r="B134" t="s">
-        <v>77</v>
-      </c>
-      <c r="F134" s="31" t="s">
-        <v>115</v>
+        <v>372</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>545</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>7</v>
@@ -6992,14 +7035,11 @@
         <v>7</v>
       </c>
       <c r="L134" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty-ŁŚ", "Sem(odstep)", 1, "1", "(1)"</v>
       </c>
       <c r="M134" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="N134" s="33" t="s">
-        <v>338</v>
+        <v>551</v>
       </c>
       <c r="O134" s="14"/>
       <c r="P134" s="14"/>
@@ -7009,29 +7049,29 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>143</v>
+        <v>546</v>
       </c>
       <c r="B135" t="s">
-        <v>20</v>
-      </c>
-      <c r="C135" t="s">
-        <v>144</v>
-      </c>
-      <c r="D135" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="G135" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E135" s="2" t="s">
+      <c r="H135" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I135" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L135" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ", "ST", 1, "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"Ty-TMo ", "SBL", 1, "1", "(2)"</v>
       </c>
       <c r="M135" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="N135" s="33" t="s">
-        <v>7</v>
+        <v>554</v>
       </c>
       <c r="O135" s="14"/>
       <c r="P135" s="14"/>
@@ -7040,30 +7080,30 @@
       <c r="S135" s="12"/>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>143</v>
+      <c r="A136" s="37" t="s">
+        <v>547</v>
       </c>
       <c r="B136" t="s">
-        <v>20</v>
-      </c>
-      <c r="C136" t="s">
-        <v>144</v>
-      </c>
-      <c r="D136" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G136" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E136" s="2" t="s">
+      <c r="H136" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I136" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="L136" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>"KZ", "ST", 2, "(1)"</v>
+        <f t="shared" si="4"/>
+        <v>"TMo-Ty", "Sem(odstęp)", 2, "1", "(1)"</v>
       </c>
       <c r="M136" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="N136" s="33" t="s">
-        <v>7</v>
+        <v>552</v>
       </c>
       <c r="O136" s="14"/>
       <c r="P136" s="14"/>
@@ -7073,29 +7113,32 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B137" t="s">
-        <v>20</v>
-      </c>
-      <c r="C137" t="s">
-        <v>144</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>8</v>
+        <v>77</v>
+      </c>
+      <c r="F137" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L137" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 3, "(2)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 1, "1", "(1)"</v>
       </c>
       <c r="M137" s="20" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="N137" s="33" t="s">
-        <v>338</v>
+        <v>7</v>
       </c>
       <c r="O137" s="14"/>
       <c r="P137" s="14"/>
@@ -7105,29 +7148,32 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B138" t="s">
-        <v>20</v>
-      </c>
-      <c r="C138" t="s">
-        <v>144</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F138" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G138" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I138" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L138" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ", "ST", 4, "(2)"</v>
+        <v>"KO-KZ", "SBL+Sem(ST)", 2, "1", "(1)"</v>
       </c>
       <c r="M138" s="20" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="N138" s="33" t="s">
-        <v>338</v>
+        <v>7</v>
       </c>
       <c r="O138" s="14"/>
       <c r="P138" s="14"/>
@@ -7137,26 +7183,32 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>527</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>527</v>
+        <v>118</v>
+      </c>
+      <c r="B139" t="s">
+        <v>77</v>
+      </c>
+      <c r="F139" s="31" t="s">
+        <v>114</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L139" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>"KZ-SG", "", 1, "1", "(3)"</v>
+        <v>"KZ-KO", "SBL+Sem(ST)", 3, "1", "(1)"</v>
       </c>
       <c r="M139" s="20" t="s">
-        <v>529</v>
+        <v>292</v>
+      </c>
+      <c r="N139" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O139" s="14"/>
       <c r="P139" s="14"/>
@@ -7166,26 +7218,32 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>528</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>528</v>
+        <v>119</v>
+      </c>
+      <c r="B140" t="s">
+        <v>77</v>
+      </c>
+      <c r="F140" s="31" t="s">
+        <v>115</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L140" s="11" t="str">
-        <f t="shared" ref="L140:L203" si="5">IF(C140="",CONCATENATE($F$1,F140,$F$1,$G$1,$F$1,B140,$F$1,$G$1,G140,$G$1,$F$1,H140,$F$1,$G$1,$F$1,$B$1,I140,$C$1,$F$1),CONCATENATE($F$1,C140,$F$1,$G$1, $F$1,B140,$F$1,$G$1,D140,$G$1,$F$1,$B$1,E140,$C$1,$F$1))</f>
-        <v>"SG-KZ", "", 2, "3", "(3)"</v>
+        <f t="shared" si="1"/>
+        <v>"KO-KZ", "SBL+Sem(ST)", 4, "1", "(1)"</v>
       </c>
       <c r="M140" s="20" t="s">
-        <v>530</v>
+        <v>293</v>
+      </c>
+      <c r="N140" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O140" s="14"/>
       <c r="P140" s="14"/>
@@ -7195,29 +7253,29 @@
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>523</v>
+        <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>67</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="G141" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C141" t="s">
+        <v>144</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="L141" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"KZ-Szb_1", "SBL", 3, "2", "(2)"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 1, "(1)"</v>
       </c>
       <c r="M141" s="20" t="s">
-        <v>531</v>
+        <v>294</v>
+      </c>
+      <c r="N141" s="33" t="s">
+        <v>7</v>
       </c>
       <c r="O141" s="14"/>
       <c r="P141" s="14"/>
@@ -7227,29 +7285,29 @@
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>524</v>
+        <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>77</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H142" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" t="s">
+        <v>144</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I142" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="L142" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"Szb-KZ_3", "SBL+Sem(ST)", 4, "1", "(3)"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 2, "(1)"</v>
       </c>
       <c r="M142" s="20" t="s">
-        <v>532</v>
+        <v>295</v>
+      </c>
+      <c r="N142" s="33" t="s">
+        <v>7</v>
       </c>
       <c r="O142" s="14"/>
       <c r="P142" s="14"/>
@@ -7258,12 +7316,30 @@
       <c r="S142" s="12"/>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143" t="s">
+        <v>144</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L143" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 3, "(2)"</v>
       </c>
       <c r="M143" s="20" t="s">
-        <v>184</v>
+        <v>296</v>
+      </c>
+      <c r="N143" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O143" s="14"/>
       <c r="P143" s="14"/>
@@ -7272,12 +7348,30 @@
       <c r="S143" s="12"/>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>20</v>
+      </c>
+      <c r="C144" t="s">
+        <v>144</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L144" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"KZ", "ST", 4, "(2)"</v>
       </c>
       <c r="M144" s="20" t="s">
-        <v>184</v>
+        <v>297</v>
+      </c>
+      <c r="N144" s="33" t="s">
+        <v>338</v>
       </c>
       <c r="O144" s="14"/>
       <c r="P144" s="14"/>
@@ -7285,13 +7379,31 @@
       <c r="R144" s="12"/>
       <c r="S144" s="12"/>
     </row>
-    <row r="145" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" t="s">
+        <v>67</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I145" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L145" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" si="1"/>
+        <v>"SG-KZ", "SBL", 1, "1", "(3)"</v>
       </c>
       <c r="M145" s="20" t="s">
-        <v>184</v>
+        <v>527</v>
       </c>
       <c r="O145" s="14"/>
       <c r="P145" s="14"/>
@@ -7299,13 +7411,31 @@
       <c r="R145" s="12"/>
       <c r="S145" s="12"/>
     </row>
-    <row r="146" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>521</v>
+      </c>
+      <c r="B146" t="s">
+        <v>77</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I146" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L146" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <f t="shared" ref="L146:L209" si="5">IF(C146="",CONCATENATE($F$1,F146,$F$1,$G$1,$F$1,B146,$F$1,$G$1,G146,$G$1,$F$1,H146,$F$1,$G$1,$F$1,$B$1,I146,$C$1,$F$1),CONCATENATE($F$1,C146,$F$1,$G$1, $F$1,B146,$F$1,$G$1,D146,$G$1,$F$1,$B$1,E146,$C$1,$F$1))</f>
+        <v>"KZ-SG", "SBL+Sem(ST)", 2, "3", "(3)"</v>
       </c>
       <c r="M146" s="20" t="s">
-        <v>184</v>
+        <v>528</v>
       </c>
       <c r="O146" s="14"/>
       <c r="P146" s="14"/>
@@ -7313,13 +7443,31 @@
       <c r="R146" s="12"/>
       <c r="S146" s="12"/>
     </row>
-    <row r="147" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>518</v>
+      </c>
+      <c r="B147" t="s">
+        <v>67</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I147" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L147" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <v>"Szb-KZ-3", "SBL", 3, "2", "(2)"</v>
       </c>
       <c r="M147" s="20" t="s">
-        <v>184</v>
+        <v>530</v>
       </c>
       <c r="O147" s="14"/>
       <c r="P147" s="14"/>
@@ -7327,13 +7475,31 @@
       <c r="R147" s="12"/>
       <c r="S147" s="12"/>
     </row>
-    <row r="148" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>519</v>
+      </c>
+      <c r="B148" t="s">
+        <v>77</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I148" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L148" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>"", "", , "", "()"</v>
+        <v>"KZ-Szb-1", "SBL+Sem(ST)", 4, "1", "(3)"</v>
       </c>
       <c r="M148" s="20" t="s">
-        <v>184</v>
+        <v>532</v>
       </c>
       <c r="O148" s="14"/>
       <c r="P148" s="14"/>
@@ -7341,7 +7507,7 @@
       <c r="R148" s="12"/>
       <c r="S148" s="12"/>
     </row>
-    <row r="149" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L149" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7355,7 +7521,7 @@
       <c r="R149" s="12"/>
       <c r="S149" s="12"/>
     </row>
-    <row r="150" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L150" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7369,7 +7535,7 @@
       <c r="R150" s="12"/>
       <c r="S150" s="12"/>
     </row>
-    <row r="151" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L151" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7383,7 +7549,7 @@
       <c r="R151" s="12"/>
       <c r="S151" s="12"/>
     </row>
-    <row r="152" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L152" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7397,7 +7563,7 @@
       <c r="R152" s="12"/>
       <c r="S152" s="12"/>
     </row>
-    <row r="153" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L153" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7405,8 +7571,13 @@
       <c r="M153" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="154" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O153" s="14"/>
+      <c r="P153" s="14"/>
+      <c r="Q153" s="12"/>
+      <c r="R153" s="12"/>
+      <c r="S153" s="12"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L154" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7414,8 +7585,13 @@
       <c r="M154" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="155" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O154" s="14"/>
+      <c r="P154" s="14"/>
+      <c r="Q154" s="12"/>
+      <c r="R154" s="12"/>
+      <c r="S154" s="12"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L155" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7423,8 +7599,13 @@
       <c r="M155" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="156" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O155" s="14"/>
+      <c r="P155" s="14"/>
+      <c r="Q155" s="12"/>
+      <c r="R155" s="12"/>
+      <c r="S155" s="12"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L156" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7432,8 +7613,13 @@
       <c r="M156" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="157" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O156" s="14"/>
+      <c r="P156" s="14"/>
+      <c r="Q156" s="12"/>
+      <c r="R156" s="12"/>
+      <c r="S156" s="12"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L157" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7441,8 +7627,13 @@
       <c r="M157" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="158" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O157" s="14"/>
+      <c r="P157" s="14"/>
+      <c r="Q157" s="12"/>
+      <c r="R157" s="12"/>
+      <c r="S157" s="12"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L158" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7450,8 +7641,13 @@
       <c r="M158" s="20" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="159" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O158" s="14"/>
+      <c r="P158" s="14"/>
+      <c r="Q158" s="12"/>
+      <c r="R158" s="12"/>
+      <c r="S158" s="12"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L159" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7460,7 +7656,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="160" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L160" s="11" t="str">
         <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
@@ -7858,7 +8054,7 @@
     </row>
     <row r="204" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L204" s="11" t="str">
-        <f t="shared" ref="L204:L267" si="6">IF(C204="",CONCATENATE($F$1,F204,$F$1,$G$1,$F$1,B204,$F$1,$G$1,G204,$G$1,$F$1,H204,$F$1,$G$1,$F$1,$B$1,I204,$C$1,$F$1),CONCATENATE($F$1,C204,$F$1,$G$1, $F$1,B204,$F$1,$G$1,D204,$G$1,$F$1,$B$1,E204,$C$1,$F$1))</f>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M204" s="20" t="s">
@@ -7867,7 +8063,7 @@
     </row>
     <row r="205" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L205" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M205" s="20" t="s">
@@ -7876,7 +8072,7 @@
     </row>
     <row r="206" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L206" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M206" s="20" t="s">
@@ -7885,7 +8081,7 @@
     </row>
     <row r="207" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L207" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M207" s="20" t="s">
@@ -7894,7 +8090,7 @@
     </row>
     <row r="208" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L208" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M208" s="20" t="s">
@@ -7903,7 +8099,7 @@
     </row>
     <row r="209" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L209" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M209" s="20" t="s">
@@ -7912,7 +8108,7 @@
     </row>
     <row r="210" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L210" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="L210:L273" si="6">IF(C210="",CONCATENATE($F$1,F210,$F$1,$G$1,$F$1,B210,$F$1,$G$1,G210,$G$1,$F$1,H210,$F$1,$G$1,$F$1,$B$1,I210,$C$1,$F$1),CONCATENATE($F$1,C210,$F$1,$G$1, $F$1,B210,$F$1,$G$1,D210,$G$1,$F$1,$B$1,E210,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M210" s="20" t="s">
@@ -8434,7 +8630,7 @@
     </row>
     <row r="268" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L268" s="11" t="str">
-        <f t="shared" ref="L268:L331" si="7">IF(C268="",CONCATENATE($F$1,F268,$F$1,$G$1,$F$1,B268,$F$1,$G$1,G268,$G$1,$F$1,H268,$F$1,$G$1,$F$1,$B$1,I268,$C$1,$F$1),CONCATENATE($F$1,C268,$F$1,$G$1, $F$1,B268,$F$1,$G$1,D268,$G$1,$F$1,$B$1,E268,$C$1,$F$1))</f>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M268" s="20" t="s">
@@ -8443,7 +8639,7 @@
     </row>
     <row r="269" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L269" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M269" s="20" t="s">
@@ -8452,7 +8648,7 @@
     </row>
     <row r="270" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L270" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M270" s="20" t="s">
@@ -8461,7 +8657,7 @@
     </row>
     <row r="271" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L271" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M271" s="20" t="s">
@@ -8470,7 +8666,7 @@
     </row>
     <row r="272" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L272" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M272" s="20" t="s">
@@ -8479,7 +8675,7 @@
     </row>
     <row r="273" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L273" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M273" s="20" t="s">
@@ -8488,7 +8684,7 @@
     </row>
     <row r="274" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L274" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L274:L337" si="7">IF(C274="",CONCATENATE($F$1,F274,$F$1,$G$1,$F$1,B274,$F$1,$G$1,G274,$G$1,$F$1,H274,$F$1,$G$1,$F$1,$B$1,I274,$C$1,$F$1),CONCATENATE($F$1,C274,$F$1,$G$1, $F$1,B274,$F$1,$G$1,D274,$G$1,$F$1,$B$1,E274,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M274" s="20" t="s">
@@ -9010,7 +9206,7 @@
     </row>
     <row r="332" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L332" s="11" t="str">
-        <f t="shared" ref="L332:L395" si="8">IF(C332="",CONCATENATE($F$1,F332,$F$1,$G$1,$F$1,B332,$F$1,$G$1,G332,$G$1,$F$1,H332,$F$1,$G$1,$F$1,$B$1,I332,$C$1,$F$1),CONCATENATE($F$1,C332,$F$1,$G$1, $F$1,B332,$F$1,$G$1,D332,$G$1,$F$1,$B$1,E332,$C$1,$F$1))</f>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M332" s="20" t="s">
@@ -9019,7 +9215,7 @@
     </row>
     <row r="333" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L333" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M333" s="20" t="s">
@@ -9028,7 +9224,7 @@
     </row>
     <row r="334" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L334" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M334" s="20" t="s">
@@ -9037,7 +9233,7 @@
     </row>
     <row r="335" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L335" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M335" s="20" t="s">
@@ -9046,7 +9242,7 @@
     </row>
     <row r="336" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L336" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M336" s="20" t="s">
@@ -9055,7 +9251,7 @@
     </row>
     <row r="337" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L337" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M337" s="20" t="s">
@@ -9064,7 +9260,7 @@
     </row>
     <row r="338" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L338" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L338:L401" si="8">IF(C338="",CONCATENATE($F$1,F338,$F$1,$G$1,$F$1,B338,$F$1,$G$1,G338,$G$1,$F$1,H338,$F$1,$G$1,$F$1,$B$1,I338,$C$1,$F$1),CONCATENATE($F$1,C338,$F$1,$G$1, $F$1,B338,$F$1,$G$1,D338,$G$1,$F$1,$B$1,E338,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M338" s="20" t="s">
@@ -9586,7 +9782,7 @@
     </row>
     <row r="396" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L396" s="11" t="str">
-        <f t="shared" ref="L396:L404" si="9">IF(C396="",CONCATENATE($F$1,F396,$F$1,$G$1,$F$1,B396,$F$1,$G$1,G396,$G$1,$F$1,H396,$F$1,$G$1,$F$1,$B$1,I396,$C$1,$F$1),CONCATENATE($F$1,C396,$F$1,$G$1, $F$1,B396,$F$1,$G$1,D396,$G$1,$F$1,$B$1,E396,$C$1,$F$1))</f>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M396" s="20" t="s">
@@ -9595,7 +9791,7 @@
     </row>
     <row r="397" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L397" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M397" s="20" t="s">
@@ -9604,7 +9800,7 @@
     </row>
     <row r="398" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L398" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M398" s="20" t="s">
@@ -9613,7 +9809,7 @@
     </row>
     <row r="399" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L399" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M399" s="20" t="s">
@@ -9622,7 +9818,7 @@
     </row>
     <row r="400" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L400" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M400" s="20" t="s">
@@ -9631,7 +9827,7 @@
     </row>
     <row r="401" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L401" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M401" s="20" t="s">
@@ -9640,7 +9836,7 @@
     </row>
     <row r="402" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L402" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="L402:L410" si="9">IF(C402="",CONCATENATE($F$1,F402,$F$1,$G$1,$F$1,B402,$F$1,$G$1,G402,$G$1,$F$1,H402,$F$1,$G$1,$F$1,$B$1,I402,$C$1,$F$1),CONCATENATE($F$1,C402,$F$1,$G$1, $F$1,B402,$F$1,$G$1,D402,$G$1,$F$1,$B$1,E402,$C$1,$F$1))</f>
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M402" s="20" t="s">
@@ -9662,6 +9858,60 @@
         <v>"", "", , "", "()"</v>
       </c>
       <c r="M404" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="405" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L405" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M405" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="406" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L406" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M406" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="407" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L407" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M407" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="408" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L408" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M408" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="409" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L409" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M409" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="410" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L410" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>"", "", , "", "()"</v>
+      </c>
+      <c r="M410" s="20" t="s">
         <v>184</v>
       </c>
     </row>
@@ -13462,6 +13712,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CD5458B81A8B2B4B92FF87D810305C72" ma:contentTypeVersion="10" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="94af6a530ab954c472b36ae778f182c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bcc645c8-4b47-4a2e-89eb-d5bbcced8466" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ef69444b0b6df3a2aca9b298e9665c5" ns3:_="">
     <xsd:import namespace="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
@@ -13645,12 +13901,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2395D0C0-9628-4C07-92CD-D40200588B84}">
   <ds:schemaRefs>
@@ -13660,6 +13910,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80CA5C0B-23D0-4CD7-AF29-D46F01A941B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BBCE1FC-4F3C-4CE6-A38A-EF0D12121C1C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13675,20 +13941,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80CA5C0B-23D0-4CD7-AF29-D46F01A941B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bcc645c8-4b47-4a2e-89eb-d5bbcced8466"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>